<commit_message>
Funciones Estadisticas y de Texto
</commit_message>
<xml_diff>
--- a/introduccion.xlsx
+++ b/introduccion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\excel-mj10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E3A5BCF-87C8-446C-A68C-F527C6A28AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662DE0D7-5AE1-4BD9-AE0E-DDD8D1846638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{141573A4-CDA2-4761-B364-CE062A8F3AE5}"/>
   </bookViews>
@@ -23,7 +23,11 @@
     <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
+    <definedName name="asist">asist.!$AG$2:$AG$11</definedName>
+    <definedName name="aus">asist.!$AF$2:$AF$11</definedName>
     <definedName name="iva_ventas">ventas!$L$2</definedName>
+    <definedName name="jornada">asist.!$AO$2</definedName>
+    <definedName name="valor_hora">asist.!$AN$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="207">
   <si>
     <t>apellido</t>
   </si>
@@ -422,9 +426,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>numeros</t>
-  </si>
-  <si>
     <t>dias</t>
   </si>
   <si>
@@ -491,13 +492,220 @@
     <t>Diciembre</t>
   </si>
   <si>
-    <t>Presentismo</t>
+    <t>fecha corta</t>
+  </si>
+  <si>
+    <t>decimales</t>
+  </si>
+  <si>
+    <t>enteros</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>factura 001</t>
+  </si>
+  <si>
+    <t>factura 012</t>
+  </si>
+  <si>
+    <t>factura 002</t>
+  </si>
+  <si>
+    <t>factura 003</t>
+  </si>
+  <si>
+    <t>factura 004</t>
+  </si>
+  <si>
+    <t>factura 005</t>
+  </si>
+  <si>
+    <t>factura 006</t>
+  </si>
+  <si>
+    <t>factura 007</t>
+  </si>
+  <si>
+    <t>factura 008</t>
+  </si>
+  <si>
+    <t>factura 009</t>
+  </si>
+  <si>
+    <t>factura 010</t>
+  </si>
+  <si>
+    <t>factura 011</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Gonzalez</t>
+  </si>
+  <si>
+    <t>Jimenez</t>
+  </si>
+  <si>
+    <t>Gimenez</t>
+  </si>
+  <si>
+    <t>Mariano</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Gabriela</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>empleado</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>01/09/22</t>
+  </si>
+  <si>
+    <t>02/09/22</t>
+  </si>
+  <si>
+    <t>03/09/22</t>
+  </si>
+  <si>
+    <t>04/09/22</t>
+  </si>
+  <si>
+    <t>05/09/22</t>
+  </si>
+  <si>
+    <t>06/09/22</t>
+  </si>
+  <si>
+    <t>07/09/22</t>
+  </si>
+  <si>
+    <t>08/09/22</t>
+  </si>
+  <si>
+    <t>09/09/22</t>
+  </si>
+  <si>
+    <t>10/09/22</t>
+  </si>
+  <si>
+    <t>11/09/22</t>
+  </si>
+  <si>
+    <t>12/09/22</t>
+  </si>
+  <si>
+    <t>13/09/22</t>
+  </si>
+  <si>
+    <t>14/09/22</t>
+  </si>
+  <si>
+    <t>15/09/22</t>
+  </si>
+  <si>
+    <t>16/09/22</t>
+  </si>
+  <si>
+    <t>17/09/22</t>
+  </si>
+  <si>
+    <t>18/09/22</t>
+  </si>
+  <si>
+    <t>19/09/22</t>
+  </si>
+  <si>
+    <t>20/09/22</t>
+  </si>
+  <si>
+    <t>21/09/22</t>
+  </si>
+  <si>
+    <t>22/09/22</t>
+  </si>
+  <si>
+    <t>23/09/22</t>
+  </si>
+  <si>
+    <t>24/09/22</t>
+  </si>
+  <si>
+    <t>25/09/22</t>
+  </si>
+  <si>
+    <t>26/09/22</t>
+  </si>
+  <si>
+    <t>27/09/22</t>
+  </si>
+  <si>
+    <t>28/09/22</t>
+  </si>
+  <si>
+    <t>29/09/22</t>
+  </si>
+  <si>
+    <t>30/09/22</t>
+  </si>
+  <si>
+    <t>Asist.</t>
+  </si>
+  <si>
+    <t>Aus.</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Inasistencia</t>
   </si>
   <si>
     <t>asistencias</t>
   </si>
   <si>
-    <t>inasistencias</t>
+    <t>mayor</t>
+  </si>
+  <si>
+    <t>menor</t>
+  </si>
+  <si>
+    <t>moda</t>
+  </si>
+  <si>
+    <t>mediana</t>
+  </si>
+  <si>
+    <t>Asist</t>
+  </si>
+  <si>
+    <t>Aus</t>
+  </si>
+  <si>
+    <t>Estadistica</t>
+  </si>
+  <si>
+    <t>sueldo</t>
+  </si>
+  <si>
+    <t>jornada</t>
+  </si>
+  <si>
+    <t>valor hora</t>
   </si>
 </sst>
 </file>
@@ -588,7 +796,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -710,6 +918,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -717,7 +934,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -807,9 +1024,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -851,6 +1065,54 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="75"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
@@ -881,37 +1143,29 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="75"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+      <alignment horizontal="left" textRotation="75"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -920,106 +1174,9 @@
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="7">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
+      <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
     </dxf>
     <dxf>
       <font>
@@ -1113,9 +1270,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
     </dxf>
     <dxf>
       <font>
@@ -1322,32 +1476,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EA1150EE-196F-4E3B-984E-194751FC9728}" name="empleados" displayName="empleados" ref="J6:J7" insertRow="1" insertRowShift="1" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="3">
-  <autoFilter ref="J6:J7" xr:uid="{EA1150EE-196F-4E3B-984E-194751FC9728}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A1BA6DD3-67CB-4A2B-AB21-8071CBEB8DD0}" name="hora" dataDxfId="2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68D78FFC-D445-4B32-A094-B9AA947FC8E6}" name="ventas" displayName="ventas" ref="D1:J19" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8" headerRowCellStyle="Moneda" dataCellStyle="Moneda">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68D78FFC-D445-4B32-A094-B9AA947FC8E6}" name="ventas" displayName="ventas" ref="D1:J19" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowCellStyle="Moneda" dataCellStyle="Moneda">
   <autoFilter ref="D1:J19" xr:uid="{68D78FFC-D445-4B32-A094-B9AA947FC8E6}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3AC5DBD6-A04E-4E7D-B94E-AE2A136DF070}" name="codigo"/>
     <tableColumn id="2" xr3:uid="{274BE5D4-57A6-4F62-AF29-6B2030F1B528}" name="cant"/>
-    <tableColumn id="3" xr3:uid="{0F9DC028-3A53-4886-8D0D-ED861C2A3CEB}" name="precio" dataDxfId="10" dataCellStyle="Moneda"/>
-    <tableColumn id="4" xr3:uid="{48AEC4E8-96DE-4725-B4D9-EBB0B8B700CF}" name="total" dataDxfId="6" dataCellStyle="Moneda">
+    <tableColumn id="3" xr3:uid="{0F9DC028-3A53-4886-8D0D-ED861C2A3CEB}" name="precio" dataDxfId="4" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{48AEC4E8-96DE-4725-B4D9-EBB0B8B700CF}" name="total" dataDxfId="3" dataCellStyle="Moneda">
       <calculatedColumnFormula>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{83C20BB9-A623-4746-82D5-84E408BD5E76}" name="iva" dataDxfId="5" dataCellStyle="Moneda">
+    <tableColumn id="5" xr3:uid="{83C20BB9-A623-4746-82D5-84E408BD5E76}" name="iva" dataDxfId="2" dataCellStyle="Moneda">
       <calculatedColumnFormula>ventas[[#This Row],[total]]*iva_ventas</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9587F797-1F6A-4699-95ED-8F390E0DAC4F}" name="precio+iva" dataDxfId="4" dataCellStyle="Moneda">
+    <tableColumn id="6" xr3:uid="{9587F797-1F6A-4699-95ED-8F390E0DAC4F}" name="precio+iva" dataDxfId="1" dataCellStyle="Moneda">
       <calculatedColumnFormula>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{710A6C7B-EF76-4F87-B111-6E49C18F5053}" name="fecha" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{710A6C7B-EF76-4F87-B111-6E49C18F5053}" name="fecha" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1650,16 +1794,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6117B3FF-61B0-4BBD-B7C7-F6DFDE9130BD}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G6"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="18" bestFit="1" customWidth="1"/>
@@ -1677,11 +1821,11 @@
       <c r="A1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="85" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>1</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>55</v>
@@ -1709,11 +1853,11 @@
       <c r="A2" s="37">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="86" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>48</v>
       </c>
       <c r="D2" s="38" t="s">
         <v>56</v>
@@ -1741,11 +1885,11 @@
       <c r="A3" s="41">
         <v>2</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="87" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>11</v>
       </c>
       <c r="D3" s="42" t="s">
         <v>57</v>
@@ -1773,11 +1917,11 @@
       <c r="A4" s="37">
         <v>3</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="45" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>26</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>58</v>
@@ -1795,7 +1939,7 @@
         <v>28</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="K4" s="9">
         <v>33346</v>
@@ -1805,11 +1949,11 @@
       <c r="A5" s="41">
         <v>4</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="87" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>32</v>
       </c>
       <c r="D5" s="42" t="s">
         <v>59</v>
@@ -1834,31 +1978,31 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="45">
+      <c r="A6" s="37">
         <v>5</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>28</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="46">
         <v>34169</v>
       </c>
-      <c r="G6" s="46" t="s">
+      <c r="G6" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="83" t="s">
+      <c r="J6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="K6" s="11">
@@ -1866,60 +2010,119 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J7" s="82"/>
+      <c r="A7" s="41">
+        <v>6</v>
+      </c>
+      <c r="B7" s="87" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="87" t="s">
+        <v>152</v>
+      </c>
+      <c r="J7" s="71" t="s">
+        <v>17</v>
+      </c>
       <c r="K7" s="12">
         <v>65000</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="J8" s="84" t="s">
-        <v>17</v>
+      <c r="A8" s="37">
+        <v>7</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="J8" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="K8" s="13">
         <v>120000</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="41">
+        <v>8</v>
+      </c>
+      <c r="B9" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="87" t="s">
+        <v>154</v>
+      </c>
       <c r="F9" s="18"/>
       <c r="H9" s="18"/>
-      <c r="J9" s="5" t="s">
-        <v>18</v>
+      <c r="J9" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="K9" s="14">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="J10" s="7" t="s">
-        <v>19</v>
+      <c r="A10" s="37">
+        <v>9</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="J10" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="K10" s="15">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="41">
+        <v>10</v>
+      </c>
+      <c r="B11" s="87" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="87" t="s">
+        <v>31</v>
+      </c>
       <c r="F11" s="18"/>
       <c r="H11" s="18"/>
-      <c r="J11" s="5" t="s">
-        <v>20</v>
+      <c r="J11" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="K11" s="17">
         <v>4294967296</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>194</v>
+      </c>
       <c r="F12" s="18"/>
       <c r="H12" s="18"/>
-      <c r="J12" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J13" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="K13" s="24" t="s">
         <v>42</v>
       </c>
@@ -1928,8 +2131,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J14" s="23" t="s">
-        <v>53</v>
+      <c r="J14" s="26" t="s">
+        <v>40</v>
       </c>
       <c r="K14" s="27" t="s">
         <v>43</v>
@@ -1939,8 +2142,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J15" s="26" t="s">
-        <v>40</v>
+      <c r="J15" s="29" t="s">
+        <v>41</v>
       </c>
       <c r="K15" s="30" t="s">
         <v>44</v>
@@ -1950,8 +2153,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J16" s="29" t="s">
-        <v>41</v>
+      <c r="J16" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="K16" s="27" t="s">
         <v>51</v>
@@ -1961,8 +2164,8 @@
       </c>
     </row>
     <row r="17" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J17" s="26" t="s">
-        <v>50</v>
+      <c r="J17" s="21" t="s">
+        <v>54</v>
       </c>
       <c r="K17" s="22" t="s">
         <v>52</v>
@@ -1971,19 +2174,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J18" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
     <row r="19" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>61</v>
+      </c>
       <c r="K19" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K20" t="s">
         <v>66</v>
@@ -1991,7 +2192,7 @@
     </row>
     <row r="21" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K21" t="s">
         <v>67</v>
@@ -1999,7 +2200,7 @@
     </row>
     <row r="22" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K22" t="s">
         <v>70</v>
@@ -2007,7 +2208,7 @@
     </row>
     <row r="23" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="K23" t="s">
         <v>69</v>
@@ -2015,7 +2216,7 @@
     </row>
     <row r="24" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="K24" t="s">
         <v>74</v>
@@ -2023,7 +2224,7 @@
     </row>
     <row r="25" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K25" t="s">
         <v>75</v>
@@ -2031,15 +2232,10 @@
     </row>
     <row r="26" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K26" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J27" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2047,202 +2243,322 @@
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.94488188976377963" bottom="0.94488188976377963" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8F921C-C865-4A35-A062-281C1CB55D2D}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:D13"/>
+      <selection activeCell="C2" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" t="s">
         <v>113</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>114</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>115</v>
       </c>
-      <c r="D1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>0.25</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
         <v>117</v>
       </c>
-      <c r="C2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="81">
+      <c r="F2" s="70">
         <v>44805</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="81">
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="70">
         <v>44806</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3" s="74">
+        <v>4.1666666666666699E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="81">
+      <c r="B4">
+        <v>0.75</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="70">
         <v>44807</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4" s="74">
+        <v>8.3333333333333301E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="81">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="70">
         <v>44808</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5" s="74">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="81">
+      <c r="B6">
+        <v>1.25</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="70">
         <v>44809</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6" s="74">
+        <v>0.16666666666666699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" s="81">
+      <c r="B7">
+        <v>1.5</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="70">
         <v>44810</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G7" s="74">
+        <v>0.20833333333333301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="81">
+      <c r="B8">
+        <v>1.75</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="70">
         <v>44811</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G8" s="74">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="81">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="70">
         <v>44812</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G9" s="74">
+        <v>0.29166666666666702</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D10" s="81">
+      <c r="B10">
+        <v>2.25</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="70">
         <v>44813</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G10" s="74">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D11" s="81">
+      <c r="B11">
+        <v>2.5</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="70">
         <v>44814</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G11" s="74">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" s="81">
+      <c r="B12">
+        <v>2.75</v>
+      </c>
+      <c r="C12" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="70">
         <v>44815</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G12" s="74">
+        <v>0.41666666666666702</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D13" s="81">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="70">
         <v>44816</v>
+      </c>
+      <c r="G13" s="74">
+        <v>0.45833333333333298</v>
       </c>
     </row>
   </sheetData>
@@ -2253,151 +2569,1444 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B38092-0CDD-4546-9420-12554152D19D}">
-  <dimension ref="A1:AG6"/>
+  <dimension ref="A1:AO15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="31" width="3.7109375" style="85" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="72" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="4.7109375" style="72" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="72" bestFit="1" customWidth="1"/>
+    <col min="13" max="31" width="4.7109375" style="72" customWidth="1"/>
+    <col min="32" max="32" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4" customWidth="1"/>
+    <col min="36" max="36" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="51" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B1" s="86">
-        <v>44805</v>
-      </c>
-      <c r="C1" s="86">
-        <v>44806</v>
-      </c>
-      <c r="D1" s="86">
-        <v>44807</v>
-      </c>
-      <c r="E1" s="86">
-        <v>44808</v>
-      </c>
-      <c r="F1" s="86">
-        <v>44809</v>
-      </c>
-      <c r="G1" s="86">
-        <v>44810</v>
-      </c>
-      <c r="H1" s="86">
-        <v>44811</v>
-      </c>
-      <c r="I1" s="86">
-        <v>44812</v>
-      </c>
-      <c r="J1" s="86">
-        <v>44813</v>
-      </c>
-      <c r="K1" s="86">
-        <v>44814</v>
-      </c>
-      <c r="L1" s="86">
-        <v>44815</v>
-      </c>
-      <c r="M1" s="86">
-        <v>44816</v>
-      </c>
-      <c r="N1" s="86">
-        <v>44817</v>
-      </c>
-      <c r="O1" s="86">
-        <v>44818</v>
-      </c>
-      <c r="P1" s="86">
-        <v>44819</v>
-      </c>
-      <c r="Q1" s="86">
-        <v>44820</v>
-      </c>
-      <c r="R1" s="86">
-        <v>44821</v>
-      </c>
-      <c r="S1" s="86">
-        <v>44822</v>
-      </c>
-      <c r="T1" s="86">
-        <v>44823</v>
-      </c>
-      <c r="U1" s="86">
-        <v>44824</v>
-      </c>
-      <c r="V1" s="86">
-        <v>44825</v>
-      </c>
-      <c r="W1" s="86">
-        <v>44826</v>
-      </c>
-      <c r="X1" s="86">
-        <v>44827</v>
-      </c>
-      <c r="Y1" s="86">
-        <v>44828</v>
-      </c>
-      <c r="Z1" s="86">
-        <v>44829</v>
-      </c>
-      <c r="AA1" s="86">
-        <v>44830</v>
-      </c>
-      <c r="AB1" s="86">
-        <v>44831</v>
-      </c>
-      <c r="AC1" s="86">
-        <v>44832</v>
-      </c>
-      <c r="AD1" s="86">
-        <v>44833</v>
-      </c>
-      <c r="AE1" s="86">
-        <v>44834</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>intro!B2</f>
-        <v>Racedo</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>intro!B3</f>
-        <v>Perez</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>intro!B4</f>
-        <v>Gomez</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f>intro!B5</f>
-        <v>Fernandez</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f>intro!B6</f>
-        <v>Lopez</v>
-      </c>
+    <row r="1" spans="1:41" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="76" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="76" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>170</v>
+      </c>
+      <c r="K1" s="76" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="76" t="s">
+        <v>172</v>
+      </c>
+      <c r="M1" s="76" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="O1" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" s="76" t="s">
+        <v>177</v>
+      </c>
+      <c r="R1" s="76" t="s">
+        <v>178</v>
+      </c>
+      <c r="S1" s="76" t="s">
+        <v>179</v>
+      </c>
+      <c r="T1" s="76" t="s">
+        <v>180</v>
+      </c>
+      <c r="U1" s="76" t="s">
+        <v>181</v>
+      </c>
+      <c r="V1" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="W1" s="76" t="s">
+        <v>183</v>
+      </c>
+      <c r="X1" s="76" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y1" s="76" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA1" s="76" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB1" s="76" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC1" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD1" s="76" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE1" s="76" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF1" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="AG1" s="99" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH1" s="99" t="s">
+        <v>204</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="AK1" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="AL1" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="AN1" s="108" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO1" s="109" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" s="79" t="str">
+        <f>_xlfn.CONCAT(intro!C2&amp;" "&amp;intro!B2)</f>
+        <v>Racedo Cristián</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="H2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="K2" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="N2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="O2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="P2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="T2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="U2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="V2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="W2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="X2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y2" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z2" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE2" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF2" s="83">
+        <f>COUNTBLANK(B2:AE2)</f>
+        <v>8</v>
+      </c>
+      <c r="AG2" s="100">
+        <f>COUNTA($B$1:$AE$1) - AF2</f>
+        <v>22</v>
+      </c>
+      <c r="AH2" s="103" cm="1">
+        <f t="array" ref="AH2">AG2*valor_hora*jornada</f>
+        <v>88000</v>
+      </c>
+      <c r="AJ2" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK2" s="105">
+        <f>AVERAGE(asist)</f>
+        <v>16.7</v>
+      </c>
+      <c r="AL2" s="106">
+        <f>AVERAGE(aus)</f>
+        <v>13.3</v>
+      </c>
+      <c r="AN2" s="110">
+        <v>500</v>
+      </c>
+      <c r="AO2" s="111">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="str">
+        <f>_xlfn.CONCAT(intro!C3&amp;" "&amp;intro!B3)</f>
+        <v>Perez Juan</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="H3" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="I3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="J3" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="K3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="N3" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="O3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="P3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="R3" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="S3" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="T3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="U3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="V3" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="W3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="X3" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z3" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD3" s="78"/>
+      <c r="AE3" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF3" s="84">
+        <f>COUNTBLANK(B3:AE3)</f>
+        <v>13</v>
+      </c>
+      <c r="AG3" s="100">
+        <f t="shared" ref="AG3:AG11" si="0">COUNTA($B$1:$AE$1) - AF3</f>
+        <v>17</v>
+      </c>
+      <c r="AH3" s="103" cm="1">
+        <f t="array" ref="AH3">AG3*valor_hora*jornada</f>
+        <v>68000</v>
+      </c>
+      <c r="AJ3" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="AK3" s="52">
+        <f>MAX(asist)</f>
+        <v>22</v>
+      </c>
+      <c r="AL3" s="53">
+        <f>MAX(aus)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="str">
+        <f>_xlfn.CONCAT(intro!C4&amp;" "&amp;intro!B4)</f>
+        <v>Gomez Gonzalo</v>
+      </c>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="N4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="O4" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="P4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q4" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="R4" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="S4" s="77"/>
+      <c r="T4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="U4" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="V4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="W4" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="X4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y4" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z4" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB4" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD4" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE4" s="77"/>
+      <c r="AF4" s="83">
+        <f>COUNTBLANK(B4:AE4)</f>
+        <v>16</v>
+      </c>
+      <c r="AG4" s="100">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AH4" s="103" cm="1">
+        <f t="array" ref="AH4">AG4*valor_hora*jornada</f>
+        <v>56000</v>
+      </c>
+      <c r="AJ4" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="AK4" s="51">
+        <f>MIN(asist)</f>
+        <v>13</v>
+      </c>
+      <c r="AL4" s="6">
+        <f>MIN(aus)</f>
+        <v>8</v>
+      </c>
+      <c r="AO4" s="73"/>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" s="80" t="str">
+        <f>_xlfn.CONCAT(intro!C5&amp;" "&amp;intro!B5)</f>
+        <v>Fernandez Daniela</v>
+      </c>
+      <c r="B5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="J5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="K5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="N5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="O5" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="P5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="R5" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="S5" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="T5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="U5" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="V5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="W5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="X5" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z5" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD5" s="78"/>
+      <c r="AE5" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF5" s="84">
+        <f>COUNTBLANK(B5:AE5)</f>
+        <v>11</v>
+      </c>
+      <c r="AG5" s="100">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AH5" s="103" cm="1">
+        <f t="array" ref="AH5">AG5*valor_hora*jornada</f>
+        <v>76000</v>
+      </c>
+      <c r="AJ5" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="AK5" s="52">
+        <f>MODE(asist)</f>
+        <v>17</v>
+      </c>
+      <c r="AL5" s="53">
+        <f>MODE(aus)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" s="79" t="str">
+        <f>_xlfn.CONCAT(intro!C6&amp;" "&amp;intro!B6)</f>
+        <v>Lopez Carla</v>
+      </c>
+      <c r="B6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="G6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="N6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="O6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="P6" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="R6" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="S6" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="T6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="U6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="V6" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="W6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="X6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y6" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z6" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB6" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE6" s="77"/>
+      <c r="AF6" s="83">
+        <f>COUNTBLANK(B6:AE6)</f>
+        <v>13</v>
+      </c>
+      <c r="AG6" s="100">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AH6" s="103" cm="1">
+        <f t="array" ref="AH6">AG6*valor_hora*jornada</f>
+        <v>68000</v>
+      </c>
+      <c r="AJ6" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="AK6" s="105">
+        <f>MEDIAN(asist)</f>
+        <v>16.5</v>
+      </c>
+      <c r="AL6" s="106">
+        <f>MEDIAN(aus)</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" s="80" t="str">
+        <f>_xlfn.CONCAT(intro!C7&amp;" "&amp;intro!B7)</f>
+        <v>Martinez Mariano</v>
+      </c>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="K7" s="78"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="N7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="O7" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="P7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="R7" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="S7" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="T7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="U7" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="V7" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="W7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="X7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z7" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB7" s="78"/>
+      <c r="AC7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD7" s="78"/>
+      <c r="AE7" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF7" s="84">
+        <f>COUNTBLANK(B7:AE7)</f>
+        <v>14</v>
+      </c>
+      <c r="AG7" s="100">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="AH7" s="103" cm="1">
+        <f t="array" ref="AH7">AG7*valor_hora*jornada</f>
+        <v>64000</v>
+      </c>
+      <c r="AJ7" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK7" s="107">
+        <f>SUM(asist)</f>
+        <v>167</v>
+      </c>
+      <c r="AL7" s="49">
+        <f>SUM(aus)</f>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" s="79" t="str">
+        <f>_xlfn.CONCAT(intro!C8&amp;" "&amp;intro!B8)</f>
+        <v>Gonzalez Gonzalo</v>
+      </c>
+      <c r="B8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="G8" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="H8" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="N8" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="O8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="P8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="R8" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="S8" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="T8" s="77"/>
+      <c r="U8" s="77"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="X8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z8" s="77"/>
+      <c r="AA8" s="77"/>
+      <c r="AB8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE8" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF8" s="83">
+        <f>COUNTBLANK(B8:AE8)</f>
+        <v>17</v>
+      </c>
+      <c r="AG8" s="100">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="AH8" s="103" cm="1">
+        <f t="array" ref="AH8">AG8*valor_hora*jornada</f>
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="80" t="str">
+        <f>_xlfn.CONCAT(intro!C9&amp;" "&amp;intro!B9)</f>
+        <v>Jimenez Jorge</v>
+      </c>
+      <c r="B9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="G9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="N9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="O9" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="P9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q9" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="R9" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="S9" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="T9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="U9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="V9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="W9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="X9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z9" s="78"/>
+      <c r="AA9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB9" s="78"/>
+      <c r="AC9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE9" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF9" s="84">
+        <f>COUNTBLANK(B9:AE9)</f>
+        <v>12</v>
+      </c>
+      <c r="AG9" s="100">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AH9" s="103" cm="1">
+        <f t="array" ref="AH9">AG9*valor_hora*jornada</f>
+        <v>72000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" s="79" t="str">
+        <f>_xlfn.CONCAT(intro!C10&amp;" "&amp;intro!B10)</f>
+        <v>Gimenez Gabriela</v>
+      </c>
+      <c r="B10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="I10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="J10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="K10" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="L10" s="77"/>
+      <c r="M10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="N10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="O10" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="P10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q10" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="R10" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="S10" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="T10" s="77"/>
+      <c r="U10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="V10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="W10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="X10" s="77"/>
+      <c r="Y10" s="77"/>
+      <c r="Z10" s="77"/>
+      <c r="AA10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD10" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE10" s="77"/>
+      <c r="AF10" s="83">
+        <f>COUNTBLANK(B10:AE10)</f>
+        <v>15</v>
+      </c>
+      <c r="AG10" s="100">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="AH10" s="103" cm="1">
+        <f t="array" ref="AH10">AG10*valor_hora*jornada</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" s="81" t="str">
+        <f>_xlfn.CONCAT(intro!C11&amp;" "&amp;intro!B11)</f>
+        <v>Lopez Laura</v>
+      </c>
+      <c r="B11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="G11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="J11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="K11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="N11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="O11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="P11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="R11" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="S11" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="T11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="U11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="V11" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="W11" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="X11" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z11" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA11" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB11" s="82"/>
+      <c r="AC11" s="82"/>
+      <c r="AD11" s="82"/>
+      <c r="AE11" s="82"/>
+      <c r="AF11" s="84">
+        <f>COUNTBLANK(B11:AE11)</f>
+        <v>14</v>
+      </c>
+      <c r="AG11" s="100">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="AH11" s="103" cm="1">
+        <f t="array" ref="AH11">AG11*valor_hora*jornada</f>
+        <v>64000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="75">
+        <f>COUNTBLANK(B2:B11)</f>
+        <v>2</v>
+      </c>
+      <c r="C12" s="75">
+        <f t="shared" ref="C12:AE12" si="1">COUNTBLANK(C2:C11)</f>
+        <v>4</v>
+      </c>
+      <c r="D12" s="75">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E12" s="75">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F12" s="75">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G12" s="75">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H12" s="75">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I12" s="75">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J12" s="75">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K12" s="75">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L12" s="75">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M12" s="75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="75">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O12" s="75">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="P12" s="75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q12" s="75">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="R12" s="75">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="S12" s="75">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="T12" s="75">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U12" s="75">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="V12" s="75">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="W12" s="75">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="X12" s="75">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Y12" s="75">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Z12" s="75">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="AA12" s="75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB12" s="75">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AC12" s="75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AD12" s="75">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AE12" s="75">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AF12" s="98">
+        <f>SUM(AF2:AF11)</f>
+        <v>133</v>
+      </c>
+      <c r="AG12" s="101">
+        <f>SUM(AG2:AG11)</f>
+        <v>167</v>
+      </c>
+      <c r="AH12" s="103"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="75">
+        <f>COUNTA($A$2:$A$11) - B12</f>
+        <v>8</v>
+      </c>
+      <c r="C13" s="75">
+        <f t="shared" ref="C13:M13" si="2">COUNTA($A$2:$A$11) - C12</f>
+        <v>6</v>
+      </c>
+      <c r="D13" s="75">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E13" s="75">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="75">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G13" s="75">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="H13" s="75">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="I13" s="75">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J13" s="75">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="K13" s="75">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="L13" s="75">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="75">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N13" s="75">
+        <f t="shared" ref="N13" si="3">COUNTA($A$2:$A$11) - N12</f>
+        <v>8</v>
+      </c>
+      <c r="O13" s="75">
+        <f t="shared" ref="O13" si="4">COUNTA($A$2:$A$11) - O12</f>
+        <v>5</v>
+      </c>
+      <c r="P13" s="75">
+        <f t="shared" ref="P13" si="5">COUNTA($A$2:$A$11) - P12</f>
+        <v>9</v>
+      </c>
+      <c r="Q13" s="75">
+        <f t="shared" ref="Q13" si="6">COUNTA($A$2:$A$11) - Q12</f>
+        <v>7</v>
+      </c>
+      <c r="R13" s="75">
+        <f t="shared" ref="R13" si="7">COUNTA($A$2:$A$11) - R12</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="75">
+        <f t="shared" ref="S13" si="8">COUNTA($A$2:$A$11) - S12</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="75">
+        <f t="shared" ref="T13" si="9">COUNTA($A$2:$A$11) - T12</f>
+        <v>8</v>
+      </c>
+      <c r="U13" s="75">
+        <f t="shared" ref="U13" si="10">COUNTA($A$2:$A$11) - U12</f>
+        <v>6</v>
+      </c>
+      <c r="V13" s="75">
+        <f t="shared" ref="V13" si="11">COUNTA($A$2:$A$11) - V12</f>
+        <v>5</v>
+      </c>
+      <c r="W13" s="75">
+        <f t="shared" ref="W13" si="12">COUNTA($A$2:$A$11) - W12</f>
+        <v>7</v>
+      </c>
+      <c r="X13" s="75">
+        <f t="shared" ref="X13" si="13">COUNTA($A$2:$A$11) - X12</f>
+        <v>6</v>
+      </c>
+      <c r="Y13" s="75">
+        <f t="shared" ref="Y13" si="14">COUNTA($A$2:$A$11) - Y12</f>
+        <v>6</v>
+      </c>
+      <c r="Z13" s="75">
+        <f t="shared" ref="Z13" si="15">COUNTA($A$2:$A$11) - Z12</f>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="75">
+        <f t="shared" ref="AA13" si="16">COUNTA($A$2:$A$11) - AA12</f>
+        <v>9</v>
+      </c>
+      <c r="AB13" s="75">
+        <f t="shared" ref="AB13" si="17">COUNTA($A$2:$A$11) - AB12</f>
+        <v>5</v>
+      </c>
+      <c r="AC13" s="75">
+        <f t="shared" ref="AC13" si="18">COUNTA($A$2:$A$11) - AC12</f>
+        <v>9</v>
+      </c>
+      <c r="AD13" s="75">
+        <f t="shared" ref="AD13" si="19">COUNTA($A$2:$A$11) - AD12</f>
+        <v>6</v>
+      </c>
+      <c r="AE13" s="75">
+        <f t="shared" ref="AE13" si="20">COUNTA($A$2:$A$11) - AE12</f>
+        <v>6</v>
+      </c>
+      <c r="AF13" s="102">
+        <f>SUM(B13:AE13)</f>
+        <v>167</v>
+      </c>
+      <c r="AG13" s="101">
+        <f>SUM(B12:AE12)</f>
+        <v>133</v>
+      </c>
+      <c r="AH13" s="103"/>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="D15" s="104"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B1:AE1 B24:AE1048576" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2421,34 +4030,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="55" t="s">
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="M1" s="55" t="s">
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="M1" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="N1" s="74" t="s">
+      <c r="N1" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -2463,7 +4072,7 @@
       <c r="D2" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="50" t="s">
         <v>82</v>
       </c>
       <c r="G2" s="23" t="s">
@@ -2478,30 +4087,30 @@
       <c r="J2" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="50" t="s">
         <v>82</v>
       </c>
       <c r="M2" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="N2" s="70" t="s">
+      <c r="N2" s="93" t="s">
         <v>95</v>
       </c>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="71"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="94"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="52">
+      <c r="B3" s="51">
         <v>8</v>
       </c>
-      <c r="C3" s="52">
+      <c r="C3" s="51">
         <v>8</v>
       </c>
-      <c r="D3" s="52">
+      <c r="D3" s="51">
         <v>12</v>
       </c>
       <c r="E3" s="6">
@@ -2511,13 +4120,13 @@
       <c r="G3" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="52">
+      <c r="H3" s="51">
         <v>8</v>
       </c>
-      <c r="I3" s="52">
+      <c r="I3" s="51">
         <v>8</v>
       </c>
-      <c r="J3" s="52">
+      <c r="J3" s="51">
         <v>12</v>
       </c>
       <c r="K3" s="6">
@@ -2528,43 +4137,43 @@
         <f>$B3+$C3+D3+A3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N3" s="72" t="s">
+      <c r="N3" s="95" t="s">
         <v>91</v>
       </c>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="73"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="96"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="52">
         <v>53</v>
       </c>
-      <c r="C4" s="53">
+      <c r="C4" s="52">
         <v>20</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="52">
         <v>14</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="53">
         <f>B4-C4-D4</f>
         <v>19</v>
       </c>
       <c r="G4" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="53">
+      <c r="H4" s="52">
         <v>53</v>
       </c>
-      <c r="I4" s="53">
+      <c r="I4" s="52">
         <v>20</v>
       </c>
-      <c r="J4" s="53">
+      <c r="J4" s="52">
         <v>14</v>
       </c>
-      <c r="K4" s="54">
+      <c r="K4" s="53">
         <f>AVERAGE(G4:J4)</f>
         <v>29</v>
       </c>
@@ -2572,24 +4181,24 @@
         <f t="array" ref="M4">$B4-$C4-D4-resta</f>
         <v>#NAME?</v>
       </c>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="68"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="91"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="52">
+      <c r="B5" s="51">
         <v>3</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="51">
         <v>8</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="51">
         <f>$B5*$C5</f>
         <v>24</v>
       </c>
@@ -2600,13 +4209,13 @@
       <c r="G5" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="52">
+      <c r="H5" s="51">
         <v>3</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="51">
         <v>8</v>
       </c>
-      <c r="J5" s="52">
+      <c r="J5" s="51">
         <f>$B5*$C5</f>
         <v>24</v>
       </c>
@@ -2618,12 +4227,12 @@
         <f>-D5*[1]pepe!A3</f>
         <v>#REF!</v>
       </c>
-      <c r="N5" s="65" t="s">
+      <c r="N5" s="88" t="s">
         <v>94</v>
       </c>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="66"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="89"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
@@ -2639,7 +4248,7 @@
         <f>$B6/$C6</f>
         <v>0.5</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="49">
         <f>B6/C6/D6</f>
         <v>1</v>
       </c>
@@ -2656,7 +4265,7 @@
         <f>$B6/$C6</f>
         <v>0.5</v>
       </c>
-      <c r="K6" s="50">
+      <c r="K6" s="49">
         <f>MOD(H6,I6)</f>
         <v>4</v>
       </c>
@@ -2664,24 +4273,24 @@
         <f>$B6/$C6/D6/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="67" t="s">
+      <c r="N6" s="90" t="s">
         <v>93</v>
       </c>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="68"/>
+      <c r="O6" s="90"/>
+      <c r="P6" s="90"/>
+      <c r="Q6" s="91"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="52">
+      <c r="B7" s="51">
         <v>2</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="51">
         <v>1</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="51">
         <v>2</v>
       </c>
       <c r="E7" s="6">
@@ -2691,13 +4300,13 @@
       <c r="G7" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="52">
+      <c r="H7" s="51">
         <v>2</v>
       </c>
-      <c r="I7" s="52">
+      <c r="I7" s="51">
         <v>1</v>
       </c>
-      <c r="J7" s="52">
+      <c r="J7" s="51">
         <v>2</v>
       </c>
       <c r="K7" s="6">
@@ -2708,12 +4317,12 @@
         <f t="array" aca="1" ref="M7" ca="1">A:A</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N7" s="65" t="s">
+      <c r="N7" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="O7" s="65"/>
-      <c r="P7" s="65"/>
-      <c r="Q7" s="66"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2740,7 +4349,7 @@
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2750,11 +4359,11 @@
     <col min="3" max="3" width="3" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="57" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="57" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="57" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="55" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.5703125" customWidth="1"/>
     <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.28515625" customWidth="1"/>
@@ -2766,7 +4375,7 @@
       <c r="A1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="61">
+      <c r="B1" s="60">
         <f>COUNT(ventas[codigo])</f>
         <v>18</v>
       </c>
@@ -2776,30 +4385,30 @@
       <c r="E1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="56" t="s">
+      <c r="J1" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="58" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="62">
+      <c r="B2" s="61">
         <f>SUM(ventas[total])</f>
         <v>287500</v>
       </c>
@@ -2809,25 +4418,25 @@
       <c r="E2">
         <v>5</v>
       </c>
-      <c r="F2" s="57">
+      <c r="F2" s="56">
         <v>5600</v>
       </c>
-      <c r="G2" s="57">
+      <c r="G2" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>28000</v>
       </c>
-      <c r="H2" s="57">
+      <c r="H2" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>5880</v>
       </c>
-      <c r="I2" s="57">
+      <c r="I2" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>33880</v>
       </c>
-      <c r="J2" s="56">
+      <c r="J2" s="55">
         <v>44824</v>
       </c>
-      <c r="L2" s="60">
+      <c r="L2" s="59">
         <v>0.21</v>
       </c>
     </row>
@@ -2835,7 +4444,7 @@
       <c r="A3" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="63">
+      <c r="B3" s="62">
         <f>MIN(ventas[total])</f>
         <v>3500</v>
       </c>
@@ -2845,30 +4454,30 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="57">
+      <c r="F3" s="56">
         <v>8000</v>
       </c>
-      <c r="G3" s="57">
+      <c r="G3" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>16000</v>
       </c>
-      <c r="H3" s="57">
+      <c r="H3" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>3360</v>
       </c>
-      <c r="I3" s="57">
+      <c r="I3" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>19360</v>
       </c>
-      <c r="J3" s="56">
+      <c r="J3" s="55">
         <v>44824</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="62">
+      <c r="B4" s="61">
         <f>MAX(ventas[total])</f>
         <v>36500</v>
       </c>
@@ -2878,30 +4487,30 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" s="57">
+      <c r="F4" s="56">
         <v>7300</v>
       </c>
-      <c r="G4" s="57">
+      <c r="G4" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>21900</v>
       </c>
-      <c r="H4" s="57">
+      <c r="H4" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>4599</v>
       </c>
-      <c r="I4" s="57">
+      <c r="I4" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>26499</v>
       </c>
-      <c r="J4" s="56">
+      <c r="J4" s="55">
         <v>44824</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="63">
+      <c r="B5" s="62">
         <f>AVERAGE(ventas[total])</f>
         <v>15972.222222222223</v>
       </c>
@@ -2911,30 +4520,30 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="57">
+      <c r="F5" s="56">
         <v>3500</v>
       </c>
-      <c r="G5" s="57">
+      <c r="G5" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>3500</v>
       </c>
-      <c r="H5" s="57">
+      <c r="H5" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>735</v>
       </c>
-      <c r="I5" s="57">
+      <c r="I5" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>4235</v>
       </c>
-      <c r="J5" s="56">
+      <c r="J5" s="55">
         <v>44825</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="64">
+      <c r="B6" s="63">
         <f>MODE(D:D)</f>
         <v>20</v>
       </c>
@@ -2944,22 +4553,22 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="57">
+      <c r="F6" s="56">
         <v>5600</v>
       </c>
-      <c r="G6" s="57">
+      <c r="G6" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>11200</v>
       </c>
-      <c r="H6" s="57">
+      <c r="H6" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>2352</v>
       </c>
-      <c r="I6" s="57">
+      <c r="I6" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>13552</v>
       </c>
-      <c r="J6" s="56">
+      <c r="J6" s="55">
         <v>44825</v>
       </c>
     </row>
@@ -2970,50 +4579,50 @@
       <c r="E7">
         <v>3</v>
       </c>
-      <c r="F7" s="57">
+      <c r="F7" s="56">
         <v>9400</v>
       </c>
-      <c r="G7" s="57">
+      <c r="G7" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>28200</v>
       </c>
-      <c r="H7" s="57">
+      <c r="H7" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>5922</v>
       </c>
-      <c r="I7" s="57">
+      <c r="I7" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>34122</v>
       </c>
-      <c r="J7" s="56">
+      <c r="J7" s="55">
         <v>44826</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="78"/>
-      <c r="B8" s="78"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="67"/>
       <c r="D8">
         <v>44</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="57">
+      <c r="F8" s="56">
         <v>8500</v>
       </c>
-      <c r="G8" s="57">
+      <c r="G8" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>8500</v>
       </c>
-      <c r="H8" s="57">
+      <c r="H8" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>1785</v>
       </c>
-      <c r="I8" s="57">
+      <c r="I8" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>10285</v>
       </c>
-      <c r="J8" s="56">
+      <c r="J8" s="55">
         <v>44827</v>
       </c>
     </row>
@@ -3024,22 +4633,22 @@
       <c r="E9">
         <v>3</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="56">
         <v>4500</v>
       </c>
-      <c r="G9" s="57">
+      <c r="G9" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>13500</v>
       </c>
-      <c r="H9" s="57">
+      <c r="H9" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>2835</v>
       </c>
-      <c r="I9" s="57">
+      <c r="I9" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>16335</v>
       </c>
-      <c r="J9" s="56">
+      <c r="J9" s="55">
         <v>44827</v>
       </c>
     </row>
@@ -3050,25 +4659,25 @@
       <c r="E10">
         <v>2</v>
       </c>
-      <c r="F10" s="57">
+      <c r="F10" s="56">
         <v>7200</v>
       </c>
-      <c r="G10" s="57">
+      <c r="G10" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>14400</v>
       </c>
-      <c r="H10" s="57">
+      <c r="H10" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>3024</v>
       </c>
-      <c r="I10" s="57">
+      <c r="I10" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>17424</v>
       </c>
-      <c r="J10" s="56">
+      <c r="J10" s="55">
         <v>44827</v>
       </c>
-      <c r="L10" s="58"/>
+      <c r="L10" s="57"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D11">
@@ -3077,25 +4686,25 @@
       <c r="E11">
         <v>5</v>
       </c>
-      <c r="F11" s="57">
+      <c r="F11" s="56">
         <v>3500</v>
       </c>
-      <c r="G11" s="57">
+      <c r="G11" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>17500</v>
       </c>
-      <c r="H11" s="57">
+      <c r="H11" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>3675</v>
       </c>
-      <c r="I11" s="57">
+      <c r="I11" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>21175</v>
       </c>
-      <c r="J11" s="56">
+      <c r="J11" s="55">
         <v>44828</v>
       </c>
-      <c r="L11" s="58"/>
+      <c r="L11" s="57"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12">
@@ -3104,25 +4713,25 @@
       <c r="E12">
         <v>4</v>
       </c>
-      <c r="F12" s="57">
+      <c r="F12" s="56">
         <v>4400</v>
       </c>
-      <c r="G12" s="57">
+      <c r="G12" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>17600</v>
       </c>
-      <c r="H12" s="57">
+      <c r="H12" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>3696</v>
       </c>
-      <c r="I12" s="57">
+      <c r="I12" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>21296</v>
       </c>
-      <c r="J12" s="56">
+      <c r="J12" s="55">
         <v>44828</v>
       </c>
-      <c r="L12" s="58"/>
+      <c r="L12" s="57"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13">
@@ -3131,25 +4740,25 @@
       <c r="E13">
         <v>3</v>
       </c>
-      <c r="F13" s="57">
+      <c r="F13" s="56">
         <v>3500</v>
       </c>
-      <c r="G13" s="57">
+      <c r="G13" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>10500</v>
       </c>
-      <c r="H13" s="57">
+      <c r="H13" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>2205</v>
       </c>
-      <c r="I13" s="57">
+      <c r="I13" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>12705</v>
       </c>
-      <c r="J13" s="56">
+      <c r="J13" s="55">
         <v>44829</v>
       </c>
-      <c r="L13" s="58"/>
+      <c r="L13" s="57"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14">
@@ -3158,25 +4767,25 @@
       <c r="E14">
         <v>2</v>
       </c>
-      <c r="F14" s="57">
+      <c r="F14" s="56">
         <v>7300</v>
       </c>
-      <c r="G14" s="57">
+      <c r="G14" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>14600</v>
       </c>
-      <c r="H14" s="57">
+      <c r="H14" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>3066</v>
       </c>
-      <c r="I14" s="57">
+      <c r="I14" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>17666</v>
       </c>
-      <c r="J14" s="56">
+      <c r="J14" s="55">
         <v>44829</v>
       </c>
-      <c r="L14" s="58"/>
+      <c r="L14" s="57"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15">
@@ -3185,25 +4794,25 @@
       <c r="E15">
         <v>3</v>
       </c>
-      <c r="F15" s="57">
+      <c r="F15" s="56">
         <v>6200</v>
       </c>
-      <c r="G15" s="57">
+      <c r="G15" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>18600</v>
       </c>
-      <c r="H15" s="57">
+      <c r="H15" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>3906</v>
       </c>
-      <c r="I15" s="57">
+      <c r="I15" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>22506</v>
       </c>
-      <c r="J15" s="56">
+      <c r="J15" s="55">
         <v>44830</v>
       </c>
-      <c r="L15" s="58"/>
+      <c r="L15" s="57"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D16">
@@ -3212,22 +4821,22 @@
       <c r="E16">
         <v>2</v>
       </c>
-      <c r="F16" s="57">
+      <c r="F16" s="56">
         <v>3500</v>
       </c>
-      <c r="G16" s="57">
+      <c r="G16" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>7000</v>
       </c>
-      <c r="H16" s="57">
+      <c r="H16" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>1470</v>
       </c>
-      <c r="I16" s="57">
+      <c r="I16" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>8470</v>
       </c>
-      <c r="J16" s="56">
+      <c r="J16" s="55">
         <v>44830</v>
       </c>
     </row>
@@ -3238,22 +4847,22 @@
       <c r="E17">
         <v>2</v>
       </c>
-      <c r="F17" s="57">
+      <c r="F17" s="56">
         <v>4400</v>
       </c>
-      <c r="G17" s="57">
+      <c r="G17" s="56">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>8800</v>
       </c>
-      <c r="H17" s="57">
+      <c r="H17" s="56">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>1848</v>
       </c>
-      <c r="I17" s="57">
+      <c r="I17" s="56">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>10648</v>
       </c>
-      <c r="J17" s="56">
+      <c r="J17" s="55">
         <v>44830</v>
       </c>
     </row>
@@ -3264,22 +4873,22 @@
       <c r="E18">
         <v>5</v>
       </c>
-      <c r="F18" s="57">
+      <c r="F18" s="56">
         <v>7300</v>
       </c>
-      <c r="G18" s="80">
+      <c r="G18" s="69">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>36500</v>
       </c>
-      <c r="H18" s="80">
+      <c r="H18" s="69">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>7665</v>
       </c>
-      <c r="I18" s="80">
+      <c r="I18" s="69">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>44165</v>
       </c>
-      <c r="J18" s="56">
+      <c r="J18" s="55">
         <v>44831</v>
       </c>
     </row>
@@ -3290,22 +4899,22 @@
       <c r="E19">
         <v>2</v>
       </c>
-      <c r="F19" s="57">
+      <c r="F19" s="56">
         <v>5600</v>
       </c>
-      <c r="G19" s="80">
+      <c r="G19" s="69">
         <f>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</f>
         <v>11200</v>
       </c>
-      <c r="H19" s="80">
+      <c r="H19" s="69">
         <f>ventas[[#This Row],[total]]*iva_ventas</f>
         <v>2352</v>
       </c>
-      <c r="I19" s="80">
+      <c r="I19" s="69">
         <f>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</f>
         <v>13552</v>
       </c>
-      <c r="J19" s="56">
+      <c r="J19" s="55">
         <v>44806</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Listas, Funciones y Formulas
</commit_message>
<xml_diff>
--- a/introduccion.xlsx
+++ b/introduccion.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\excel-x15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3DB1F2-14DB-456A-A763-772918DD3A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53260A3B-4575-4E6D-AE88-C9D8B7E8AB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A9001261-B951-436E-B7B5-5E5DD5F49FEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="1" r:id="rId1"/>
+    <sheet name="listas" sheetId="2" r:id="rId2"/>
+    <sheet name="f(x)" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -33,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="108">
   <si>
     <t>Tipos</t>
   </si>
@@ -166,22 +190,214 @@
   </si>
   <si>
     <t>1:1;</t>
+  </si>
+  <si>
+    <t>dias</t>
+  </si>
+  <si>
+    <t>meses</t>
+  </si>
+  <si>
+    <t>horas</t>
+  </si>
+  <si>
+    <t>minutos</t>
+  </si>
+  <si>
+    <t>fechas</t>
+  </si>
+  <si>
+    <t>texto</t>
+  </si>
+  <si>
+    <t>fac_A001</t>
+  </si>
+  <si>
+    <t>fac_A002</t>
+  </si>
+  <si>
+    <t>fac_A003</t>
+  </si>
+  <si>
+    <t>fac_A004</t>
+  </si>
+  <si>
+    <t>fac_A005</t>
+  </si>
+  <si>
+    <t>fac_A006</t>
+  </si>
+  <si>
+    <t>fac_A007</t>
+  </si>
+  <si>
+    <t>fac_A008</t>
+  </si>
+  <si>
+    <t>fac_A009</t>
+  </si>
+  <si>
+    <t>fac_A010</t>
+  </si>
+  <si>
+    <t>miercoles</t>
+  </si>
+  <si>
+    <t>jueves</t>
+  </si>
+  <si>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t>sábado</t>
+  </si>
+  <si>
+    <t>domingo</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t>miércoles</t>
+  </si>
+  <si>
+    <t>octubre</t>
+  </si>
+  <si>
+    <t>noviembre</t>
+  </si>
+  <si>
+    <t>diciembre</t>
+  </si>
+  <si>
+    <t>enero</t>
+  </si>
+  <si>
+    <t>febrero</t>
+  </si>
+  <si>
+    <t>marzo</t>
+  </si>
+  <si>
+    <t>abril</t>
+  </si>
+  <si>
+    <t>mayo</t>
+  </si>
+  <si>
+    <t>junio</t>
+  </si>
+  <si>
+    <t>julio</t>
+  </si>
+  <si>
+    <t>fac_A011</t>
+  </si>
+  <si>
+    <t>fac_A012</t>
+  </si>
+  <si>
+    <t>agosto</t>
+  </si>
+  <si>
+    <t>septiembre</t>
+  </si>
+  <si>
+    <t>DEC</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>formulas</t>
+  </si>
+  <si>
+    <t>funciones</t>
+  </si>
+  <si>
+    <t>errores</t>
+  </si>
+  <si>
+    <t>operaciones matematicas que utilizan valores numericos de referencia, los cuales deben ser utilizables, ya que de lo contrario arrojara un error</t>
+  </si>
+  <si>
+    <t>palabras reservadas que se utilizan para realizar alguna operación en particular, trabajan con rangos y suelen ignorar aquellos valores no utilizables</t>
+  </si>
+  <si>
+    <t>Mensaje que aparece dentro de la celda y que hace referencia a un problema ocurrido con la formula o funcion correspondiente</t>
+  </si>
+  <si>
+    <t>operaciones</t>
+  </si>
+  <si>
+    <t>valor a</t>
+  </si>
+  <si>
+    <t>valor b</t>
+  </si>
+  <si>
+    <t>resultado</t>
+  </si>
+  <si>
+    <t>suma</t>
+  </si>
+  <si>
+    <t>resta</t>
+  </si>
+  <si>
+    <t>producto</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>SUMA()</t>
+  </si>
+  <si>
+    <t>CONTAR()</t>
+  </si>
+  <si>
+    <t>PRODUCTO()</t>
+  </si>
+  <si>
+    <t>RESIDUO()</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>significado</t>
+  </si>
+  <si>
+    <t>El valor utilizado no se reconoce</t>
+  </si>
+  <si>
+    <t>El tipo de dato utilizado es incorrecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No se encuentra la celda o rango </t>
+  </si>
+  <si>
+    <t>No se puede dividir entre 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="7">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="166" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="171" formatCode="[$-2C0A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="169" formatCode="[$-2C0A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +413,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
@@ -205,25 +428,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -235,6 +451,50 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -262,19 +522,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
       <top style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </top>
@@ -314,13 +561,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -328,84 +595,120 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="4" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="20" fontId="1" fillId="6" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="3"/>
+    <xf numFmtId="20" fontId="1" fillId="8" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="1" fillId="11" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+  <cellStyles count="10">
+    <cellStyle name="40% - Énfasis6" xfId="1" builtinId="51"/>
+    <cellStyle name="60% - Énfasis1" xfId="2" builtinId="32"/>
+    <cellStyle name="60% - Énfasis2" xfId="3" builtinId="36"/>
+    <cellStyle name="Énfasis1" xfId="4" builtinId="29"/>
+    <cellStyle name="Énfasis2" xfId="5" builtinId="33"/>
+    <cellStyle name="Énfasis3" xfId="6" builtinId="37"/>
+    <cellStyle name="Énfasis6" xfId="7" builtinId="49"/>
+    <cellStyle name="Moneda" xfId="8" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="9" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -418,6 +721,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="hoja1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -716,11 +1032,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881F7159-F93E-4F91-852E-B17342539A20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +1044,8 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
@@ -971,4 +1288,873 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V13"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:A65536"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="21" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="L1" s="40">
+        <v>0.4</v>
+      </c>
+      <c r="M1" s="40">
+        <v>0.6</v>
+      </c>
+      <c r="N1" s="40">
+        <v>0.8</v>
+      </c>
+      <c r="O1" s="40">
+        <v>1</v>
+      </c>
+      <c r="P1" s="40">
+        <v>1.2</v>
+      </c>
+      <c r="Q1" s="40">
+        <v>1.4</v>
+      </c>
+      <c r="R1" s="40">
+        <v>1.6</v>
+      </c>
+      <c r="S1" s="40">
+        <v>1.8</v>
+      </c>
+      <c r="T1" s="40">
+        <v>2</v>
+      </c>
+      <c r="U1" s="40">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V1" s="40">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="45">
+        <v>0.625</v>
+      </c>
+      <c r="G2" s="47">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="H2" s="49">
+        <v>44853</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="R2" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="S2" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="V2" s="41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="40">
+        <v>0.4</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="45">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G3" s="47">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H3" s="49">
+        <v>44854</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="S3" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="40">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="45">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="G4" s="47">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="H4" s="49">
+        <v>44855</v>
+      </c>
+      <c r="J4" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="P4" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q4" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="R4" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="S4" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="T4" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="U4" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="V4" s="43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="40">
+        <v>0.8</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="45">
+        <v>0.75</v>
+      </c>
+      <c r="G5" s="47">
+        <v>2.77777777777777E-2</v>
+      </c>
+      <c r="H5" s="49">
+        <v>44856</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="45">
+        <v>0.625</v>
+      </c>
+      <c r="L5" s="45">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M5" s="45">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="N5" s="45">
+        <v>0.75</v>
+      </c>
+      <c r="O5" s="45">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="P5" s="45">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="Q5" s="45">
+        <v>0.875</v>
+      </c>
+      <c r="R5" s="45">
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="S5" s="45">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="T5" s="45">
+        <v>1</v>
+      </c>
+      <c r="U5" s="45">
+        <v>1.0416666666666701</v>
+      </c>
+      <c r="V5" s="45">
+        <v>1.0833333333333299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="40">
+        <v>1</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="45">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="G6" s="47">
+        <v>3.4722222222222203E-2</v>
+      </c>
+      <c r="H6" s="49">
+        <v>44857</v>
+      </c>
+      <c r="J6" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="47">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="L6" s="47">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="M6" s="47">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="N6" s="47">
+        <v>2.77777777777777E-2</v>
+      </c>
+      <c r="O6" s="47">
+        <v>3.4722222222222203E-2</v>
+      </c>
+      <c r="P6" s="47">
+        <v>4.1666666666666602E-2</v>
+      </c>
+      <c r="Q6" s="47">
+        <v>4.8611111111111098E-2</v>
+      </c>
+      <c r="R6" s="47">
+        <v>5.5555555555555497E-2</v>
+      </c>
+      <c r="S6" s="47">
+        <v>6.25E-2</v>
+      </c>
+      <c r="T6" s="47">
+        <v>6.9444444444444406E-2</v>
+      </c>
+      <c r="U6" s="47">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="V6" s="47">
+        <v>8.3333333333333301E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="40">
+        <v>1.2</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="45">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="G7" s="47">
+        <v>4.1666666666666602E-2</v>
+      </c>
+      <c r="H7" s="49">
+        <v>44858</v>
+      </c>
+      <c r="J7" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="49">
+        <v>44853</v>
+      </c>
+      <c r="L7" s="49">
+        <v>44854</v>
+      </c>
+      <c r="M7" s="49">
+        <v>44855</v>
+      </c>
+      <c r="N7" s="49">
+        <v>44856</v>
+      </c>
+      <c r="O7" s="49">
+        <v>44857</v>
+      </c>
+      <c r="P7" s="49">
+        <v>44858</v>
+      </c>
+      <c r="Q7" s="49">
+        <v>44859</v>
+      </c>
+      <c r="R7" s="49">
+        <v>44860</v>
+      </c>
+      <c r="S7" s="49">
+        <v>44861</v>
+      </c>
+      <c r="T7" s="49">
+        <v>44862</v>
+      </c>
+      <c r="U7" s="49">
+        <v>44863</v>
+      </c>
+      <c r="V7" s="49">
+        <v>44864</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="40">
+        <v>1.4</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="45">
+        <v>0.875</v>
+      </c>
+      <c r="G8" s="47">
+        <v>4.8611111111111098E-2</v>
+      </c>
+      <c r="H8" s="49">
+        <v>44859</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="40">
+        <v>1.6</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="45">
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="G9" s="47">
+        <v>5.5555555555555497E-2</v>
+      </c>
+      <c r="H9" s="49">
+        <v>44860</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="40">
+        <v>1.8</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="45">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="G10" s="47">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H10" s="49">
+        <v>44861</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="40">
+        <v>2</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="45">
+        <v>1</v>
+      </c>
+      <c r="G11" s="47">
+        <v>6.9444444444444406E-2</v>
+      </c>
+      <c r="H11" s="49">
+        <v>44862</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="40">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="45">
+        <v>1.0416666666666701</v>
+      </c>
+      <c r="G12" s="47">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="H12" s="49">
+        <v>44863</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="40">
+        <v>2.4</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="45">
+        <v>1.0833333333333299</v>
+      </c>
+      <c r="G13" s="47">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H13" s="49">
+        <v>44864</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="2.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="2.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="F1" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="K1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="31">
+        <v>5</v>
+      </c>
+      <c r="C3" s="31">
+        <v>2</v>
+      </c>
+      <c r="D3" s="57">
+        <f>B3+C3</f>
+        <v>7</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="31">
+        <v>5</v>
+      </c>
+      <c r="H3" s="31">
+        <v>2</v>
+      </c>
+      <c r="I3" s="57">
+        <f>SUM(F3:H3)</f>
+        <v>7</v>
+      </c>
+      <c r="K3" s="11" t="e" cm="1">
+        <f t="array" ref="K3">personal</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L3" s="57" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="32">
+        <v>7</v>
+      </c>
+      <c r="C4" s="32">
+        <v>4</v>
+      </c>
+      <c r="D4" s="58">
+        <f>B4-C4</f>
+        <v>3</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="32">
+        <v>7</v>
+      </c>
+      <c r="H4" s="32">
+        <v>4</v>
+      </c>
+      <c r="I4" s="58">
+        <f>COUNT(F4:H4)</f>
+        <v>2</v>
+      </c>
+      <c r="K4" s="14" t="e">
+        <f>F4+G4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L4" s="58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="31">
+        <v>3</v>
+      </c>
+      <c r="C5" s="31">
+        <v>2</v>
+      </c>
+      <c r="D5" s="57">
+        <f>B5*C5</f>
+        <v>6</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="31">
+        <v>3</v>
+      </c>
+      <c r="H5" s="31">
+        <v>2</v>
+      </c>
+      <c r="I5" s="57">
+        <f>PRODUCT(F5:H5)</f>
+        <v>6</v>
+      </c>
+      <c r="K5" s="11" t="e">
+        <f>[1]hoja1!A4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L5" s="57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="6">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="56">
+        <f>B6/C6</f>
+        <v>2</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="6">
+        <v>6</v>
+      </c>
+      <c r="H6" s="6">
+        <v>3</v>
+      </c>
+      <c r="I6" s="56">
+        <f>MOD(G6,H6)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="55" t="e">
+        <f>10/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L6" s="56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Filtros y Reemplazar palabras
</commit_message>
<xml_diff>
--- a/introduccion.xlsx
+++ b/introduccion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\excel-mj10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABE31F6-D1F8-4AF4-8A13-1D5349354E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0D0CA4-08D8-473F-9E85-805C8C9824C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="410" firstSheet="4" activeTab="6" xr2:uid="{141573A4-CDA2-4761-B364-CE062A8F3AE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="410" activeTab="1" xr2:uid="{141573A4-CDA2-4761-B364-CE062A8F3AE5}"/>
   </bookViews>
   <sheets>
     <sheet name="menu" sheetId="8" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="326">
   <si>
     <t>apellido</t>
   </si>
@@ -855,9 +855,6 @@
     <t>mm</t>
   </si>
   <si>
-    <t>producto</t>
-  </si>
-  <si>
     <t>stock</t>
   </si>
   <si>
@@ -1078,6 +1075,12 @@
   </si>
   <si>
     <t>reponer</t>
+  </si>
+  <si>
+    <t>articulo</t>
+  </si>
+  <si>
+    <t>Larralde</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1096,7 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="174" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="170" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1603,6 +1606,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1636,23 +1656,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Énfasis1" xfId="3" builtinId="30"/>
@@ -1667,780 +1670,7 @@
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="83">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkVertical">
-          <fgColor theme="9"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="174" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="174" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="79">
     <dxf>
       <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
     </dxf>
@@ -2554,6 +1784,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
@@ -3503,6 +2748,714 @@
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="[$-2C0A]hh:mm:ss\ AM/PM;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -4741,8 +4694,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>182217</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="categoria">
@@ -4765,7 +4718,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -4819,8 +4772,8 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>182217</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="proveedor">
@@ -4843,7 +4796,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -5077,60 +5030,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A66DC253-4297-42E8-811E-51DF8355CE68}" name="empleados" displayName="empleados" ref="D1:S12" totalsRowCount="1" headerRowDxfId="82" dataDxfId="81" tableBorderDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A66DC253-4297-42E8-811E-51DF8355CE68}" name="empleados" displayName="empleados" ref="D1:S12" totalsRowCount="1" headerRowDxfId="78" dataDxfId="77" tableBorderDxfId="76">
   <autoFilter ref="D1:S11" xr:uid="{A66DC253-4297-42E8-811E-51DF8355CE68}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{AD2BFDC6-9212-4AF1-A883-4F5292CC8670}" name="EMPLEADO" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="20">
+    <tableColumn id="1" xr3:uid="{AD2BFDC6-9212-4AF1-A883-4F5292CC8670}" name="EMPLEADO" totalsRowFunction="custom" dataDxfId="75" totalsRowDxfId="74">
       <calculatedColumnFormula>asistencia!A2</calculatedColumnFormula>
       <totalsRowFormula>COUNTA(empleados[EMPLEADO])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{9941B11B-F67E-4F32-82D2-B86FEB7E9F6E}" name="APELLIDO" dataDxfId="35" totalsRowDxfId="19">
+    <tableColumn id="8" xr3:uid="{9941B11B-F67E-4F32-82D2-B86FEB7E9F6E}" name="APELLIDO" dataDxfId="73" totalsRowDxfId="72">
       <calculatedColumnFormula>LEFT(empleados[[#This Row],[EMPLEADO]], empleados[[#This Row],[CHAR]] - 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{DEEF5E54-5054-45B9-B8EE-A5D09A981708}" name="NOMBRE" dataDxfId="34" totalsRowDxfId="18">
+    <tableColumn id="9" xr3:uid="{DEEF5E54-5054-45B9-B8EE-A5D09A981708}" name="NOMBRE" dataDxfId="71" totalsRowDxfId="70">
       <calculatedColumnFormula>RIGHT(empleados[[#This Row],[EMPLEADO]], empleados[[#This Row],[LARGO]] - (LEN(empleados[[#This Row],[APELLIDO]]) + 2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{4F40C219-FD97-4CAB-B243-ECFB4C424AFF}" name="CUIL" dataDxfId="33" totalsRowDxfId="17">
+    <tableColumn id="2" xr3:uid="{4F40C219-FD97-4CAB-B243-ECFB4C424AFF}" name="CUIL" dataDxfId="69" totalsRowDxfId="68">
       <calculatedColumnFormula>introduccion!D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{62C6429F-DFB5-4F13-9C8C-F4F9A8B2BFF4}" name="TIPO" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="16">
+    <tableColumn id="3" xr3:uid="{62C6429F-DFB5-4F13-9C8C-F4F9A8B2BFF4}" name="TIPO" totalsRowFunction="custom" dataDxfId="67" totalsRowDxfId="66">
       <calculatedColumnFormula>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</calculatedColumnFormula>
       <totalsRowFormula>MODE(empleados[TIPO])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{19B71444-5CC4-45F1-8222-5A8DBAD1B101}" name="DOCUMENTO" dataDxfId="31" totalsRowDxfId="15" dataCellStyle="Millares">
+    <tableColumn id="4" xr3:uid="{19B71444-5CC4-45F1-8222-5A8DBAD1B101}" name="DOCUMENTO" dataDxfId="65" totalsRowDxfId="64" dataCellStyle="Millares">
       <calculatedColumnFormula>MID(empleados[[#This Row],[CUIL]],4,8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E886725E-39BE-415C-979A-1175DA7DBC26}" name="VERIF" dataDxfId="30" totalsRowDxfId="14">
+    <tableColumn id="5" xr3:uid="{E886725E-39BE-415C-979A-1175DA7DBC26}" name="VERIF" dataDxfId="63" totalsRowDxfId="62">
       <calculatedColumnFormula>RIGHT(empleados[[#This Row],[CUIL]],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C0528248-53F2-4B9A-B0FC-54DAC797D388}" name="CHAR" dataDxfId="29" totalsRowDxfId="13">
+    <tableColumn id="6" xr3:uid="{C0528248-53F2-4B9A-B0FC-54DAC797D388}" name="CHAR" dataDxfId="61" totalsRowDxfId="60">
       <calculatedColumnFormula>FIND(separador,empleados[[#This Row],[EMPLEADO]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7ACF23E0-4058-4529-87E3-89A0F10EDEE7}" name="LARGO" totalsRowFunction="max" dataDxfId="28" totalsRowDxfId="12">
+    <tableColumn id="7" xr3:uid="{7ACF23E0-4058-4529-87E3-89A0F10EDEE7}" name="LARGO" totalsRowFunction="max" dataDxfId="59" totalsRowDxfId="58">
       <calculatedColumnFormula>LEN(empleados[[#This Row],[EMPLEADO]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C0311DC3-1821-46B4-BAF2-F825CC93183C}" name="NACIMIENTO" dataDxfId="27" totalsRowDxfId="11">
+    <tableColumn id="10" xr3:uid="{C0311DC3-1821-46B4-BAF2-F825CC93183C}" name="NACIMIENTO" dataDxfId="57" totalsRowDxfId="56">
       <calculatedColumnFormula>introduccion!E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{C5EF39FB-0151-4B57-8F47-0735E6F3917B}" name="EDAD" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="10">
+    <tableColumn id="11" xr3:uid="{C5EF39FB-0151-4B57-8F47-0735E6F3917B}" name="EDAD" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="54">
       <calculatedColumnFormula>(datos_hoy - empleados[[#This Row],[NACIMIENTO]]) / 365</calculatedColumnFormula>
       <totalsRowFormula>AVERAGE(empleados[EDAD])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A025954B-A9FF-49BA-A580-9FA9F8B233C2}" name="AÑOS" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="9">
+    <tableColumn id="12" xr3:uid="{A025954B-A9FF-49BA-A580-9FA9F8B233C2}" name="AÑOS" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="52">
       <calculatedColumnFormula>$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</calculatedColumnFormula>
       <totalsRowFormula>AVERAGE(empleados[AÑOS])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{2EAA4AB1-5773-4D81-8119-48C5A0C08F69}" name="entrada" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="8">
+    <tableColumn id="13" xr3:uid="{2EAA4AB1-5773-4D81-8119-48C5A0C08F69}" name="entrada" totalsRowFunction="custom" dataDxfId="51" totalsRowDxfId="50">
       <totalsRowFormula>MEDIAN(empleados[entrada])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{341FD674-15E1-44A6-B749-E39DAB5E740A}" name="salida" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="7">
+    <tableColumn id="14" xr3:uid="{341FD674-15E1-44A6-B749-E39DAB5E740A}" name="salida" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="48">
       <totalsRowFormula>MEDIAN(empleados[salida])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{3C8E616C-CB51-4D78-B9BD-1CEB59933A8F}" name="H" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="6">
+    <tableColumn id="17" xr3:uid="{3C8E616C-CB51-4D78-B9BD-1CEB59933A8F}" name="H" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="46">
       <calculatedColumnFormula>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</calculatedColumnFormula>
       <totalsRowFormula>AVERAGE(empleados[H])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{21F27A62-D009-45A5-A9C8-60FBC9C20CF7}" name="mm" totalsRowFunction="custom" dataDxfId="21">
+    <tableColumn id="18" xr3:uid="{21F27A62-D009-45A5-A9C8-60FBC9C20CF7}" name="mm" totalsRowFunction="custom" dataDxfId="45">
       <calculatedColumnFormula>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</calculatedColumnFormula>
       <totalsRowFormula>AVERAGE(empleados[mm])</totalsRowFormula>
     </tableColumn>
@@ -5140,109 +5093,109 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EB255E47-4E76-4E15-B9ED-DABF169EDCDF}" name="asistencia" displayName="asistencia" ref="A1:AH12" totalsRowCount="1" tableBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EB255E47-4E76-4E15-B9ED-DABF169EDCDF}" name="asistencia" displayName="asistencia" ref="A1:AH12" totalsRowCount="1" tableBorderDxfId="44">
   <autoFilter ref="A1:AH11" xr:uid="{EB255E47-4E76-4E15-B9ED-DABF169EDCDF}"/>
   <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{FFB40CFD-2FB0-4BA8-9AD2-20F41FFE821E}" name="EMPLEADOS" totalsRowLabel="Total" dataDxfId="78">
+    <tableColumn id="1" xr3:uid="{FFB40CFD-2FB0-4BA8-9AD2-20F41FFE821E}" name="EMPLEADOS" totalsRowLabel="Total" dataDxfId="43">
       <calculatedColumnFormula>_xlfn.CONCAT(introduccion!C2&amp;", "&amp;introduccion!B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7CD2E68C-D07C-4635-B469-EBACA13F9D82}" name="01/09/22" totalsRowFunction="custom" dataDxfId="77">
+    <tableColumn id="2" xr3:uid="{7CD2E68C-D07C-4635-B469-EBACA13F9D82}" name="01/09/22" totalsRowFunction="custom" dataDxfId="42">
       <totalsRowFormula>COUNTA($A$2:$A$11) - COUNTBLANK(B2:B11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6782312C-2AED-4FF2-B804-F6EC82A9B619}" name="02/09/22" totalsRowFunction="custom" dataDxfId="76">
+    <tableColumn id="3" xr3:uid="{6782312C-2AED-4FF2-B804-F6EC82A9B619}" name="02/09/22" totalsRowFunction="custom" dataDxfId="41">
       <totalsRowFormula>COUNTBLANK(C2:C11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6A44F1E-D0D7-4343-B875-865BCF5DE859}" name="03/09/22" totalsRowFunction="custom" dataDxfId="75">
+    <tableColumn id="4" xr3:uid="{C6A44F1E-D0D7-4343-B875-865BCF5DE859}" name="03/09/22" totalsRowFunction="custom" dataDxfId="40">
       <totalsRowFormula>COUNTBLANK(D2:D11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1B6A406D-2E5A-4E52-9AF8-9BBB22029492}" name="04/09/22" totalsRowFunction="custom" dataDxfId="74">
+    <tableColumn id="5" xr3:uid="{1B6A406D-2E5A-4E52-9AF8-9BBB22029492}" name="04/09/22" totalsRowFunction="custom" dataDxfId="39">
       <totalsRowFormula>COUNTBLANK(E2:E11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8B393F8F-816E-412F-8868-DE374FC96561}" name="05/09/22" totalsRowFunction="custom" dataDxfId="73">
+    <tableColumn id="6" xr3:uid="{8B393F8F-816E-412F-8868-DE374FC96561}" name="05/09/22" totalsRowFunction="custom" dataDxfId="38">
       <totalsRowFormula>COUNTBLANK(F2:F11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A3EEB526-D699-481A-B321-F21F70B94670}" name="06/09/22" totalsRowFunction="custom" dataDxfId="72">
+    <tableColumn id="7" xr3:uid="{A3EEB526-D699-481A-B321-F21F70B94670}" name="06/09/22" totalsRowFunction="custom" dataDxfId="37">
       <totalsRowFormula>COUNTBLANK(G2:G11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{F22C56C5-CB9F-40AD-81E2-33C9F951222A}" name="07/09/22" totalsRowFunction="custom" dataDxfId="71">
+    <tableColumn id="8" xr3:uid="{F22C56C5-CB9F-40AD-81E2-33C9F951222A}" name="07/09/22" totalsRowFunction="custom" dataDxfId="36">
       <totalsRowFormula>COUNTBLANK(H2:H11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{73160653-73D2-4AB2-AF88-C92D864411FC}" name="08/09/22" totalsRowFunction="custom" dataDxfId="70">
+    <tableColumn id="9" xr3:uid="{73160653-73D2-4AB2-AF88-C92D864411FC}" name="08/09/22" totalsRowFunction="custom" dataDxfId="35">
       <totalsRowFormula>COUNTBLANK(I2:I11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{81C87D0C-5C80-4ADA-9017-C1883C821D5F}" name="09/09/22" totalsRowFunction="custom" dataDxfId="69">
+    <tableColumn id="10" xr3:uid="{81C87D0C-5C80-4ADA-9017-C1883C821D5F}" name="09/09/22" totalsRowFunction="custom" dataDxfId="34">
       <totalsRowFormula>COUNTBLANK(J2:J11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{C452CA74-AE98-4EBE-B4AF-BFD228DE07E6}" name="10/09/22" totalsRowFunction="custom" dataDxfId="68">
+    <tableColumn id="11" xr3:uid="{C452CA74-AE98-4EBE-B4AF-BFD228DE07E6}" name="10/09/22" totalsRowFunction="custom" dataDxfId="33">
       <totalsRowFormula>COUNTBLANK(K2:K11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{58FFD11A-AC9F-4F8E-8D7E-4F699E6FFAF5}" name="11/09/22" totalsRowFunction="custom" dataDxfId="67">
+    <tableColumn id="12" xr3:uid="{58FFD11A-AC9F-4F8E-8D7E-4F699E6FFAF5}" name="11/09/22" totalsRowFunction="custom" dataDxfId="32">
       <totalsRowFormula>COUNTBLANK(L2:L11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EF89081F-FC50-4D28-B748-E215BB32BF49}" name="12/09/22" totalsRowFunction="custom" dataDxfId="66">
+    <tableColumn id="13" xr3:uid="{EF89081F-FC50-4D28-B748-E215BB32BF49}" name="12/09/22" totalsRowFunction="custom" dataDxfId="31">
       <totalsRowFormula>COUNTBLANK(M2:M11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{9DC5AC26-133B-4292-A104-18BDAEB4A78F}" name="13/09/22" totalsRowFunction="custom" dataDxfId="65">
+    <tableColumn id="14" xr3:uid="{9DC5AC26-133B-4292-A104-18BDAEB4A78F}" name="13/09/22" totalsRowFunction="custom" dataDxfId="30">
       <totalsRowFormula>COUNTBLANK(N2:N11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{A771D892-D621-46F4-9537-1B265C8E9A36}" name="14/09/22" totalsRowFunction="custom" dataDxfId="64">
+    <tableColumn id="15" xr3:uid="{A771D892-D621-46F4-9537-1B265C8E9A36}" name="14/09/22" totalsRowFunction="custom" dataDxfId="29">
       <totalsRowFormula>COUNTBLANK(O2:O11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{1F6F4D30-C62F-4312-9A7E-E1167AF5A05D}" name="15/09/22" totalsRowFunction="custom" dataDxfId="63">
+    <tableColumn id="16" xr3:uid="{1F6F4D30-C62F-4312-9A7E-E1167AF5A05D}" name="15/09/22" totalsRowFunction="custom" dataDxfId="28">
       <totalsRowFormula>COUNTBLANK(P2:P11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{2D64B6B4-4A83-487B-9E69-1C35894B58C5}" name="16/09/22" totalsRowFunction="custom" dataDxfId="62">
+    <tableColumn id="17" xr3:uid="{2D64B6B4-4A83-487B-9E69-1C35894B58C5}" name="16/09/22" totalsRowFunction="custom" dataDxfId="27">
       <totalsRowFormula>COUNTBLANK(Q2:Q11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{66F27389-1D9E-4B4E-AF0D-D7BB5386C4E2}" name="17/09/22" totalsRowFunction="custom" dataDxfId="61">
+    <tableColumn id="18" xr3:uid="{66F27389-1D9E-4B4E-AF0D-D7BB5386C4E2}" name="17/09/22" totalsRowFunction="custom" dataDxfId="26">
       <totalsRowFormula>COUNTBLANK(R2:R11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{DC182874-F7F9-48B4-BA09-DF7DD0C46D02}" name="18/09/22" totalsRowFunction="custom" dataDxfId="60">
+    <tableColumn id="19" xr3:uid="{DC182874-F7F9-48B4-BA09-DF7DD0C46D02}" name="18/09/22" totalsRowFunction="custom" dataDxfId="25">
       <totalsRowFormula>COUNTBLANK(S2:S11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{F211762A-904D-400D-8935-B6F09029DC73}" name="19/09/22" totalsRowFunction="custom" dataDxfId="59">
+    <tableColumn id="20" xr3:uid="{F211762A-904D-400D-8935-B6F09029DC73}" name="19/09/22" totalsRowFunction="custom" dataDxfId="24">
       <totalsRowFormula>COUNTBLANK(T2:T11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{3C17D129-9505-44DD-BBE0-ABF261CDE4BE}" name="20/09/22" totalsRowFunction="custom" dataDxfId="58">
+    <tableColumn id="21" xr3:uid="{3C17D129-9505-44DD-BBE0-ABF261CDE4BE}" name="20/09/22" totalsRowFunction="custom" dataDxfId="23">
       <totalsRowFormula>COUNTBLANK(U2:U11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{3839BFCA-649A-4DA4-9CC5-401179A69E94}" name="21/09/22" totalsRowFunction="custom" dataDxfId="57">
+    <tableColumn id="22" xr3:uid="{3839BFCA-649A-4DA4-9CC5-401179A69E94}" name="21/09/22" totalsRowFunction="custom" dataDxfId="22">
       <totalsRowFormula>COUNTBLANK(V2:V11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{CFA2F06A-8EE1-416E-910B-59D7BC443557}" name="22/09/22" totalsRowFunction="custom" dataDxfId="56">
+    <tableColumn id="23" xr3:uid="{CFA2F06A-8EE1-416E-910B-59D7BC443557}" name="22/09/22" totalsRowFunction="custom" dataDxfId="21">
       <totalsRowFormula>COUNTBLANK(W2:W11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{FF543CC5-D769-401F-B919-8083D15D1E25}" name="23/09/22" totalsRowFunction="custom" dataDxfId="55">
+    <tableColumn id="24" xr3:uid="{FF543CC5-D769-401F-B919-8083D15D1E25}" name="23/09/22" totalsRowFunction="custom" dataDxfId="20">
       <totalsRowFormula>COUNTBLANK(X2:X11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{19785421-596B-4949-9FE6-AC04B9A8A0B8}" name="24/09/22" totalsRowFunction="custom" dataDxfId="54">
+    <tableColumn id="25" xr3:uid="{19785421-596B-4949-9FE6-AC04B9A8A0B8}" name="24/09/22" totalsRowFunction="custom" dataDxfId="19">
       <totalsRowFormula>COUNTBLANK(Y2:Y11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{77DCF724-123A-4A25-A01B-4B525F174906}" name="25/09/22" totalsRowFunction="custom" dataDxfId="53">
+    <tableColumn id="26" xr3:uid="{77DCF724-123A-4A25-A01B-4B525F174906}" name="25/09/22" totalsRowFunction="custom" dataDxfId="18">
       <totalsRowFormula>COUNTBLANK(Z2:Z11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{AC499496-18FA-4796-B6D1-8CB8B24D4635}" name="26/09/22" totalsRowFunction="custom" dataDxfId="52">
+    <tableColumn id="27" xr3:uid="{AC499496-18FA-4796-B6D1-8CB8B24D4635}" name="26/09/22" totalsRowFunction="custom" dataDxfId="17">
       <totalsRowFormula>COUNTBLANK(AA2:AA11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{D4ED44DE-9137-499F-85ED-BCD7ECD9A1EA}" name="27/09/22" totalsRowFunction="custom" dataDxfId="51">
+    <tableColumn id="28" xr3:uid="{D4ED44DE-9137-499F-85ED-BCD7ECD9A1EA}" name="27/09/22" totalsRowFunction="custom" dataDxfId="16">
       <totalsRowFormula>COUNTBLANK(AB2:AB11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{E385E835-FA8B-4251-9748-1E5B35CF35FC}" name="28/09/22" totalsRowFunction="custom" dataDxfId="50">
+    <tableColumn id="29" xr3:uid="{E385E835-FA8B-4251-9748-1E5B35CF35FC}" name="28/09/22" totalsRowFunction="custom" dataDxfId="15">
       <totalsRowFormula>COUNTBLANK(AC2:AC11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{0D4459DA-D655-4F90-A83C-FD20F4AD3F3E}" name="29/09/22" totalsRowFunction="custom" dataDxfId="49">
+    <tableColumn id="30" xr3:uid="{0D4459DA-D655-4F90-A83C-FD20F4AD3F3E}" name="29/09/22" totalsRowFunction="custom" dataDxfId="14">
       <totalsRowFormula>COUNTBLANK(AD2:AD11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{32451497-3DB8-4B31-ADDF-E9C1A2599C46}" name="30/09/22" totalsRowFunction="custom" dataDxfId="48">
+    <tableColumn id="31" xr3:uid="{32451497-3DB8-4B31-ADDF-E9C1A2599C46}" name="30/09/22" totalsRowFunction="custom" dataDxfId="13">
       <totalsRowFormula>COUNTBLANK(AE2:AE11)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{3DD562B3-0719-4D45-8340-C2ACEA5547A7}" name="Aus." totalsRowFunction="sum" dataDxfId="47">
+    <tableColumn id="32" xr3:uid="{3DD562B3-0719-4D45-8340-C2ACEA5547A7}" name="Aus." totalsRowFunction="sum" dataDxfId="12">
       <calculatedColumnFormula>COUNTBLANK(B2:AE2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{FB33E439-6F10-43AB-8172-EF83DE1E891A}" name="Asist." totalsRowFunction="sum" dataDxfId="46">
+    <tableColumn id="33" xr3:uid="{FB33E439-6F10-43AB-8172-EF83DE1E891A}" name="Asist." totalsRowFunction="sum" dataDxfId="11">
       <calculatedColumnFormula>COUNTA($B$1:$AE$1) - AF2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{0D66ED41-FA53-4A07-8873-DA93C74A6065}" name="sueldo" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44">
+    <tableColumn id="34" xr3:uid="{0D66ED41-FA53-4A07-8873-DA93C74A6065}" name="sueldo" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula array="1">AG2*valor_hora*jornada</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5258,12 +5211,12 @@
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{219F5B7E-D8F1-4D71-A7D2-CE12FFC1D082}" name="codigo"/>
-    <tableColumn id="2" xr3:uid="{466C7B34-0A79-4FE0-9FA5-31DEDBF20899}" name="producto"/>
+    <tableColumn id="2" xr3:uid="{466C7B34-0A79-4FE0-9FA5-31DEDBF20899}" name="articulo"/>
     <tableColumn id="3" xr3:uid="{A6107C8B-32BB-4ED2-B185-CE6F6D183D48}" name="stock"/>
     <tableColumn id="4" xr3:uid="{767E403C-9FBB-4BCE-9865-EF64259A8953}" name="precio" dataCellStyle="Moneda"/>
     <tableColumn id="7" xr3:uid="{A963D90F-E9F8-4FC4-8718-F7142DB1FD23}" name="categoria"/>
     <tableColumn id="5" xr3:uid="{94932026-CF59-4D21-87B8-F036F8B814F6}" name="proveedor"/>
-    <tableColumn id="6" xr3:uid="{07D0E63B-FFEF-4AD5-9550-F9F71A9F24CB}" name="reponer" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{07D0E63B-FFEF-4AD5-9550-F9F71A9F24CB}" name="reponer" dataDxfId="7">
       <calculatedColumnFormula>Tabla2[[#This Row],[stock]]&lt;=5000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5272,22 +5225,22 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68D78FFC-D445-4B32-A094-B9AA947FC8E6}" name="ventas" displayName="ventas" ref="D1:J19" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" headerRowCellStyle="Moneda" dataCellStyle="Moneda">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68D78FFC-D445-4B32-A094-B9AA947FC8E6}" name="ventas" displayName="ventas" ref="D1:J19" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowCellStyle="Moneda" dataCellStyle="Moneda">
   <autoFilter ref="D1:J19" xr:uid="{68D78FFC-D445-4B32-A094-B9AA947FC8E6}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3AC5DBD6-A04E-4E7D-B94E-AE2A136DF070}" name="codigo"/>
     <tableColumn id="2" xr3:uid="{274BE5D4-57A6-4F62-AF29-6B2030F1B528}" name="cant"/>
-    <tableColumn id="3" xr3:uid="{0F9DC028-3A53-4886-8D0D-ED861C2A3CEB}" name="precio" dataDxfId="41" dataCellStyle="Moneda"/>
-    <tableColumn id="4" xr3:uid="{48AEC4E8-96DE-4725-B4D9-EBB0B8B700CF}" name="total" dataDxfId="40" dataCellStyle="Moneda">
+    <tableColumn id="3" xr3:uid="{0F9DC028-3A53-4886-8D0D-ED861C2A3CEB}" name="precio" dataDxfId="4" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{48AEC4E8-96DE-4725-B4D9-EBB0B8B700CF}" name="total" dataDxfId="3" dataCellStyle="Moneda">
       <calculatedColumnFormula>ventas[[#This Row],[cant]]*ventas[[#This Row],[precio]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{83C20BB9-A623-4746-82D5-84E408BD5E76}" name="iva" dataDxfId="39" dataCellStyle="Moneda">
+    <tableColumn id="5" xr3:uid="{83C20BB9-A623-4746-82D5-84E408BD5E76}" name="iva" dataDxfId="2" dataCellStyle="Moneda">
       <calculatedColumnFormula>ventas[[#This Row],[total]]*iva_ventas</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9587F797-1F6A-4699-95ED-8F390E0DAC4F}" name="precio+iva" dataDxfId="38" dataCellStyle="Moneda">
+    <tableColumn id="6" xr3:uid="{9587F797-1F6A-4699-95ED-8F390E0DAC4F}" name="precio+iva" dataDxfId="1" dataCellStyle="Moneda">
       <calculatedColumnFormula>ventas[[#This Row],[total]]+ventas[[#This Row],[iva]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{710A6C7B-EF76-4F87-B111-6E49C18F5053}" name="fecha" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{710A6C7B-EF76-4F87-B111-6E49C18F5053}" name="fecha" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5596,7 +5549,7 @@
   <dimension ref="A2:F5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5605,12 +5558,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="134" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="121"/>
+      <c r="A3" s="134"/>
       <c r="B3" s="120" t="s">
         <v>234</v>
       </c>
@@ -5628,12 +5581,12 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="134" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="121"/>
+      <c r="A5" s="134"/>
       <c r="B5" s="120" t="s">
         <v>238</v>
       </c>
@@ -5675,9 +5628,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6117B3FF-61B0-4BBD-B7C7-F6DFDE9130BD}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G11"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5974,7 +5927,7 @@
         <v>157</v>
       </c>
       <c r="C11" s="82" t="s">
-        <v>30</v>
+        <v>325</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>212</v>
@@ -6731,7 +6684,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6749,31 +6702,31 @@
       <c r="A1" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="126" t="s">
+      <c r="B1" s="139" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
       <c r="F1" s="48"/>
       <c r="G1" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="126" t="s">
+      <c r="H1" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
       <c r="M1" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="131" t="s">
+      <c r="N1" s="144" t="s">
         <v>100</v>
       </c>
-      <c r="O1" s="131"/>
-      <c r="P1" s="131"/>
-      <c r="Q1" s="131"/>
+      <c r="O1" s="144"/>
+      <c r="P1" s="144"/>
+      <c r="Q1" s="144"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -6809,12 +6762,12 @@
       <c r="M2" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="N2" s="127" t="s">
+      <c r="N2" s="140" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="127"/>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="128"/>
+      <c r="O2" s="140"/>
+      <c r="P2" s="140"/>
+      <c r="Q2" s="141"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -6853,12 +6806,12 @@
         <f>$B3+$C3+D3+A3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N3" s="129" t="s">
+      <c r="N3" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="O3" s="129"/>
-      <c r="P3" s="129"/>
-      <c r="Q3" s="130"/>
+      <c r="O3" s="142"/>
+      <c r="P3" s="142"/>
+      <c r="Q3" s="143"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
@@ -6897,12 +6850,12 @@
         <f t="array" ref="M4">$B4-$C4-D4-resta</f>
         <v>#NAME?</v>
       </c>
-      <c r="N4" s="124" t="s">
+      <c r="N4" s="137" t="s">
         <v>91</v>
       </c>
-      <c r="O4" s="124"/>
-      <c r="P4" s="124"/>
-      <c r="Q4" s="125"/>
+      <c r="O4" s="137"/>
+      <c r="P4" s="137"/>
+      <c r="Q4" s="138"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
@@ -6943,12 +6896,12 @@
         <f>-D5*[1]pepe!A3</f>
         <v>#REF!</v>
       </c>
-      <c r="N5" s="122" t="s">
+      <c r="N5" s="135" t="s">
         <v>93</v>
       </c>
-      <c r="O5" s="122"/>
-      <c r="P5" s="122"/>
-      <c r="Q5" s="123"/>
+      <c r="O5" s="135"/>
+      <c r="P5" s="135"/>
+      <c r="Q5" s="136"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
@@ -6989,12 +6942,12 @@
         <f>$B6/$C6/D6/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="124" t="s">
+      <c r="N6" s="137" t="s">
         <v>92</v>
       </c>
-      <c r="O6" s="124"/>
-      <c r="P6" s="124"/>
-      <c r="Q6" s="125"/>
+      <c r="O6" s="137"/>
+      <c r="P6" s="137"/>
+      <c r="Q6" s="138"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -7033,12 +6986,12 @@
         <f t="array" aca="1" ref="M7" ca="1">A:A</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N7" s="122" t="s">
+      <c r="N7" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="O7" s="122"/>
-      <c r="P7" s="122"/>
-      <c r="Q7" s="123"/>
+      <c r="O7" s="135"/>
+      <c r="P7" s="135"/>
+      <c r="Q7" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -7085,8 +7038,8 @@
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.42578125" customWidth="1"/>
-    <col min="16" max="17" width="13.28515625" style="142" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.5703125" style="139" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.28515625" style="131" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" style="128" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -7134,13 +7087,13 @@
       <c r="O1" s="104" t="s">
         <v>230</v>
       </c>
-      <c r="P1" s="140" t="s">
+      <c r="P1" s="129" t="s">
         <v>246</v>
       </c>
-      <c r="Q1" s="140" t="s">
+      <c r="Q1" s="129" t="s">
         <v>247</v>
       </c>
-      <c r="R1" s="138" t="s">
+      <c r="R1" s="127" t="s">
         <v>248</v>
       </c>
       <c r="S1" s="104" t="s">
@@ -7164,7 +7117,7 @@
         <f>introduccion!D2</f>
         <v>20-35336446-5</v>
       </c>
-      <c r="H2" s="137">
+      <c r="H2" s="126">
         <f>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</f>
         <v>20</v>
       </c>
@@ -7196,17 +7149,17 @@
         <f ca="1">$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</f>
         <v>31</v>
       </c>
-      <c r="P2" s="141">
+      <c r="P2" s="130">
         <v>0.42708333333333331</v>
       </c>
-      <c r="Q2" s="141">
+      <c r="Q2" s="130">
         <v>0.5</v>
       </c>
       <c r="R2" s="108">
         <f>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</f>
         <v>2</v>
       </c>
-      <c r="S2" s="135">
+      <c r="S2" s="124">
         <f>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</f>
         <v>45</v>
       </c>
@@ -7234,7 +7187,7 @@
         <f>introduccion!D3</f>
         <v>20-43128323-1</v>
       </c>
-      <c r="H3" s="137">
+      <c r="H3" s="126">
         <f>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</f>
         <v>20</v>
       </c>
@@ -7266,17 +7219,17 @@
         <f ca="1">$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</f>
         <v>25</v>
       </c>
-      <c r="P3" s="141">
+      <c r="P3" s="130">
         <v>0.41666666666666669</v>
       </c>
-      <c r="Q3" s="141">
+      <c r="Q3" s="130">
         <v>0.50694444444444442</v>
       </c>
       <c r="R3" s="108">
         <f>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</f>
         <v>2</v>
       </c>
-      <c r="S3" s="135">
+      <c r="S3" s="124">
         <f>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</f>
         <v>10</v>
       </c>
@@ -7306,7 +7259,7 @@
         <f>introduccion!D4</f>
         <v>20-30283492-6</v>
       </c>
-      <c r="H4" s="137">
+      <c r="H4" s="126">
         <f>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</f>
         <v>20</v>
       </c>
@@ -7338,17 +7291,17 @@
         <f ca="1">$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</f>
         <v>35</v>
       </c>
-      <c r="P4" s="141">
+      <c r="P4" s="130">
         <v>0.41666666666666669</v>
       </c>
-      <c r="Q4" s="141">
+      <c r="Q4" s="130">
         <v>0.5</v>
       </c>
       <c r="R4" s="108">
         <f>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</f>
         <v>2</v>
       </c>
-      <c r="S4" s="135">
+      <c r="S4" s="124">
         <f>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</f>
         <v>0</v>
       </c>
@@ -7357,9 +7310,9 @@
       <c r="A5" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="B5" s="132">
+      <c r="B5" s="121">
         <f ca="1">NOW()</f>
-        <v>44845.496178703703</v>
+        <v>44845.499446759262</v>
       </c>
       <c r="D5" s="52" t="str">
         <f>asistencia!A5</f>
@@ -7377,7 +7330,7 @@
         <f>introduccion!D5</f>
         <v>27-33230498-2</v>
       </c>
-      <c r="H5" s="137">
+      <c r="H5" s="126">
         <f>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</f>
         <v>27</v>
       </c>
@@ -7409,17 +7362,17 @@
         <f ca="1">$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</f>
         <v>33</v>
       </c>
-      <c r="P5" s="141">
+      <c r="P5" s="130">
         <v>0.4375</v>
       </c>
-      <c r="Q5" s="141">
+      <c r="Q5" s="130">
         <v>0.53125</v>
       </c>
       <c r="R5" s="108">
         <f>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</f>
         <v>2</v>
       </c>
-      <c r="S5" s="135">
+      <c r="S5" s="124">
         <f>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</f>
         <v>15</v>
       </c>
@@ -7448,7 +7401,7 @@
         <f>introduccion!D6</f>
         <v>27-38578293-4</v>
       </c>
-      <c r="H6" s="137">
+      <c r="H6" s="126">
         <f>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</f>
         <v>27</v>
       </c>
@@ -7480,17 +7433,17 @@
         <f ca="1">$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</f>
         <v>29</v>
       </c>
-      <c r="P6" s="141">
+      <c r="P6" s="130">
         <v>0.42708333333333331</v>
       </c>
-      <c r="Q6" s="141">
+      <c r="Q6" s="130">
         <v>0.50694444444444442</v>
       </c>
       <c r="R6" s="108">
         <f>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</f>
         <v>2</v>
       </c>
-      <c r="S6" s="135">
+      <c r="S6" s="124">
         <f>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</f>
         <v>55</v>
       </c>
@@ -7519,7 +7472,7 @@
         <f>introduccion!D7</f>
         <v>20-28234973-3</v>
       </c>
-      <c r="H7" s="137">
+      <c r="H7" s="126">
         <f>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</f>
         <v>20</v>
       </c>
@@ -7551,17 +7504,17 @@
         <f ca="1">$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</f>
         <v>35</v>
       </c>
-      <c r="P7" s="141">
+      <c r="P7" s="130">
         <v>0.41666666666666669</v>
       </c>
-      <c r="Q7" s="141">
+      <c r="Q7" s="130">
         <v>0.5</v>
       </c>
       <c r="R7" s="108">
         <f>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</f>
         <v>2</v>
       </c>
-      <c r="S7" s="135">
+      <c r="S7" s="124">
         <f>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</f>
         <v>0</v>
       </c>
@@ -7590,7 +7543,7 @@
         <f>introduccion!D8</f>
         <v>20-39128371-1</v>
       </c>
-      <c r="H8" s="137">
+      <c r="H8" s="126">
         <f>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</f>
         <v>20</v>
       </c>
@@ -7622,17 +7575,17 @@
         <f ca="1">$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</f>
         <v>28</v>
       </c>
-      <c r="P8" s="141">
+      <c r="P8" s="130">
         <v>0.375</v>
       </c>
-      <c r="Q8" s="141">
+      <c r="Q8" s="130">
         <v>0.54166666666666663</v>
       </c>
       <c r="R8" s="108">
         <f>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</f>
         <v>4</v>
       </c>
-      <c r="S8" s="135">
+      <c r="S8" s="124">
         <f>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</f>
         <v>0</v>
       </c>
@@ -7661,7 +7614,7 @@
         <f>introduccion!D9</f>
         <v>20-45019105-2</v>
       </c>
-      <c r="H9" s="137">
+      <c r="H9" s="126">
         <f>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</f>
         <v>20</v>
       </c>
@@ -7693,17 +7646,17 @@
         <f ca="1">$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</f>
         <v>19</v>
       </c>
-      <c r="P9" s="141">
+      <c r="P9" s="130">
         <v>0.4375</v>
       </c>
-      <c r="Q9" s="141">
+      <c r="Q9" s="130">
         <v>0.50694444444444442</v>
       </c>
       <c r="R9" s="108">
         <f>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</f>
         <v>2</v>
       </c>
-      <c r="S9" s="135">
+      <c r="S9" s="124">
         <f>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</f>
         <v>40</v>
       </c>
@@ -7714,7 +7667,7 @@
       </c>
       <c r="B10" s="6">
         <f ca="1">MINUTE(B5)</f>
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D10" s="51" t="str">
         <f>asistencia!A10</f>
@@ -7732,7 +7685,7 @@
         <f>introduccion!D10</f>
         <v>27-31203948-8</v>
       </c>
-      <c r="H10" s="137">
+      <c r="H10" s="126">
         <f>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</f>
         <v>27</v>
       </c>
@@ -7764,17 +7717,17 @@
         <f ca="1">$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</f>
         <v>36</v>
       </c>
-      <c r="P10" s="141">
+      <c r="P10" s="130">
         <v>0.42708333333333331</v>
       </c>
-      <c r="Q10" s="141">
+      <c r="Q10" s="130">
         <v>0.54166666666666663</v>
       </c>
       <c r="R10" s="108">
         <f>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</f>
         <v>3</v>
       </c>
-      <c r="S10" s="135">
+      <c r="S10" s="124">
         <f>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</f>
         <v>45</v>
       </c>
@@ -7785,15 +7738,15 @@
       </c>
       <c r="B11" s="49">
         <f ca="1">SECOND(B5)</f>
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D11" s="52" t="str">
         <f>asistencia!A11</f>
-        <v>Lopez, Laura</v>
+        <v>Larralde, Laura</v>
       </c>
       <c r="E11" s="52" t="str">
         <f>LEFT(empleados[[#This Row],[EMPLEADO]], empleados[[#This Row],[CHAR]] - 1)</f>
-        <v>Lopez</v>
+        <v>Larralde</v>
       </c>
       <c r="F11" s="52" t="str">
         <f>RIGHT(empleados[[#This Row],[EMPLEADO]], empleados[[#This Row],[LARGO]] - (LEN(empleados[[#This Row],[APELLIDO]]) + 2))</f>
@@ -7803,7 +7756,7 @@
         <f>introduccion!D11</f>
         <v>27-30192834-4</v>
       </c>
-      <c r="H11" s="137">
+      <c r="H11" s="126">
         <f>_xlfn.NUMBERVALUE(LEFT(empleados[[#This Row],[CUIL]],2))</f>
         <v>27</v>
       </c>
@@ -7817,11 +7770,11 @@
       </c>
       <c r="K11" s="52">
         <f>FIND(separador,empleados[[#This Row],[EMPLEADO]])</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L11" s="52">
         <f>LEN(empleados[[#This Row],[EMPLEADO]])</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M11" s="105">
         <f>introduccion!E11</f>
@@ -7835,17 +7788,17 @@
         <f ca="1">$B$6 - YEAR(empleados[[#This Row],[NACIMIENTO]])</f>
         <v>37</v>
       </c>
-      <c r="P11" s="141">
+      <c r="P11" s="130">
         <v>0.41666666666666669</v>
       </c>
-      <c r="Q11" s="141">
+      <c r="Q11" s="130">
         <v>0.53125</v>
       </c>
       <c r="R11" s="108">
         <f>HOUR(empleados[[#This Row],[salida]]) - HOUR(empleados[[#This Row],[entrada]])</f>
         <v>2</v>
       </c>
-      <c r="S11" s="135">
+      <c r="S11" s="124">
         <f>MINUTE(empleados[[#This Row],[salida]]-empleados[[#This Row],[entrada]])</f>
         <v>45</v>
       </c>
@@ -7855,21 +7808,21 @@
         <f>COUNTA(empleados[EMPLEADO])</f>
         <v>10</v>
       </c>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="122"/>
       <c r="G12" s="52"/>
-      <c r="H12" s="136">
+      <c r="H12" s="125">
         <f>MODE(empleados[TIPO])</f>
         <v>20</v>
       </c>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="133"/>
-      <c r="L12" s="133">
+      <c r="I12" s="122"/>
+      <c r="J12" s="122"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="122">
         <f>SUBTOTAL(104,empleados[LARGO])</f>
         <v>18</v>
       </c>
-      <c r="M12" s="134"/>
+      <c r="M12" s="123"/>
       <c r="N12" s="106">
         <f ca="1">AVERAGE(empleados[EDAD])</f>
         <v>31.11698630136986</v>
@@ -7878,15 +7831,15 @@
         <f ca="1">AVERAGE(empleados[AÑOS])</f>
         <v>30.8</v>
       </c>
-      <c r="P12" s="142">
+      <c r="P12" s="131">
         <f>MEDIAN(empleados[entrada])</f>
         <v>0.421875</v>
       </c>
-      <c r="Q12" s="142">
+      <c r="Q12" s="131">
         <f>MEDIAN(empleados[salida])</f>
         <v>0.50694444444444442</v>
       </c>
-      <c r="R12" s="139">
+      <c r="R12" s="128">
         <f>AVERAGE(empleados[H])</f>
         <v>2.2999999999999998</v>
       </c>
@@ -9007,7 +8960,7 @@
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="str">
         <f>_xlfn.CONCAT(introduccion!C11&amp;", "&amp;introduccion!B11)</f>
-        <v>Lopez, Laura</v>
+        <v>Larralde, Laura</v>
       </c>
       <c r="B11" s="77" t="s">
         <v>158</v>
@@ -9322,8 +9275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366DFCC1-0733-4BBC-8410-31F61302687F}">
   <dimension ref="C1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E12"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9350,37 +9303,37 @@
         <v>97</v>
       </c>
       <c r="D1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E1" t="s">
         <v>250</v>
-      </c>
-      <c r="E1" t="s">
-        <v>251</v>
       </c>
       <c r="F1" s="56" t="s">
         <v>107</v>
       </c>
       <c r="G1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K1" t="s">
-        <v>274</v>
-      </c>
-      <c r="L1" s="143" t="s">
+        <v>273</v>
+      </c>
+      <c r="L1" s="132" t="s">
+        <v>271</v>
+      </c>
+      <c r="M1" t="s">
         <v>272</v>
       </c>
-      <c r="M1" t="s">
-        <v>273</v>
-      </c>
       <c r="N1" t="s">
+        <v>286</v>
+      </c>
+      <c r="O1" t="s">
         <v>287</v>
-      </c>
-      <c r="O1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="2" spans="3:15" x14ac:dyDescent="0.25">
@@ -9388,7 +9341,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E2">
         <v>300</v>
@@ -9397,28 +9350,28 @@
         <v>3800</v>
       </c>
       <c r="G2" t="s">
+        <v>254</v>
+      </c>
+      <c r="H2" t="s">
         <v>255</v>
-      </c>
-      <c r="H2" t="s">
-        <v>256</v>
       </c>
       <c r="I2" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>1</v>
       </c>
-      <c r="K2" s="121" t="s">
-        <v>270</v>
+      <c r="K2" s="134" t="s">
+        <v>269</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M2" t="s">
-        <v>281</v>
-      </c>
-      <c r="N2" s="144" t="s">
-        <v>289</v>
-      </c>
-      <c r="O2" s="144">
+        <v>280</v>
+      </c>
+      <c r="N2" s="133" t="s">
+        <v>288</v>
+      </c>
+      <c r="O2" s="133">
         <v>2</v>
       </c>
     </row>
@@ -9427,7 +9380,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E3">
         <v>1200</v>
@@ -9436,27 +9389,27 @@
         <v>25800</v>
       </c>
       <c r="G3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I3" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>1</v>
       </c>
-      <c r="K3" s="121"/>
+      <c r="K3" s="134"/>
       <c r="L3" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M3" t="s">
-        <v>282</v>
-      </c>
-      <c r="N3" s="144" t="s">
+        <v>281</v>
+      </c>
+      <c r="N3" s="133" t="s">
+        <v>288</v>
+      </c>
+      <c r="O3" s="133" t="s">
         <v>289</v>
-      </c>
-      <c r="O3" s="144" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.25">
@@ -9464,7 +9417,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E4">
         <v>5000</v>
@@ -9473,26 +9426,26 @@
         <v>17800</v>
       </c>
       <c r="G4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H4" t="s">
         <v>260</v>
-      </c>
-      <c r="H4" t="s">
-        <v>261</v>
       </c>
       <c r="I4" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>1</v>
       </c>
-      <c r="K4" s="121"/>
+      <c r="K4" s="134"/>
       <c r="L4" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M4" t="s">
-        <v>283</v>
-      </c>
-      <c r="N4" s="144" t="s">
-        <v>289</v>
-      </c>
-      <c r="O4" s="144">
+        <v>282</v>
+      </c>
+      <c r="N4" s="133" t="s">
+        <v>288</v>
+      </c>
+      <c r="O4" s="133">
         <v>1</v>
       </c>
     </row>
@@ -9501,7 +9454,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E5">
         <v>2000</v>
@@ -9510,26 +9463,26 @@
         <v>8500</v>
       </c>
       <c r="G5" t="s">
+        <v>262</v>
+      </c>
+      <c r="H5" t="s">
         <v>263</v>
-      </c>
-      <c r="H5" t="s">
-        <v>264</v>
       </c>
       <c r="I5" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>1</v>
       </c>
-      <c r="K5" s="121"/>
+      <c r="K5" s="134"/>
       <c r="L5" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M5" t="s">
-        <v>284</v>
-      </c>
-      <c r="N5" s="144" t="s">
-        <v>289</v>
-      </c>
-      <c r="O5" s="144">
+        <v>283</v>
+      </c>
+      <c r="N5" s="133" t="s">
+        <v>288</v>
+      </c>
+      <c r="O5" s="133">
         <v>1.2</v>
       </c>
     </row>
@@ -9538,7 +9491,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E6">
         <v>8500</v>
@@ -9547,27 +9500,27 @@
         <v>5000</v>
       </c>
       <c r="G6" t="s">
+        <v>262</v>
+      </c>
+      <c r="H6" t="s">
         <v>263</v>
-      </c>
-      <c r="H6" t="s">
-        <v>264</v>
       </c>
       <c r="I6" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>0</v>
       </c>
-      <c r="K6" s="121"/>
+      <c r="K6" s="134"/>
       <c r="L6" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M6" t="s">
-        <v>285</v>
-      </c>
-      <c r="N6" s="144" t="s">
-        <v>289</v>
-      </c>
-      <c r="O6" s="144" t="s">
-        <v>291</v>
+        <v>284</v>
+      </c>
+      <c r="N6" s="133" t="s">
+        <v>288</v>
+      </c>
+      <c r="O6" s="133" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.25">
@@ -9575,7 +9528,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E7">
         <v>15000</v>
@@ -9584,27 +9537,27 @@
         <v>105000</v>
       </c>
       <c r="G7" t="s">
+        <v>266</v>
+      </c>
+      <c r="H7" t="s">
         <v>267</v>
-      </c>
-      <c r="H7" t="s">
-        <v>268</v>
       </c>
       <c r="I7" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>0</v>
       </c>
-      <c r="K7" s="121"/>
+      <c r="K7" s="134"/>
       <c r="L7" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M7" t="s">
-        <v>286</v>
-      </c>
-      <c r="N7" s="144" t="s">
-        <v>289</v>
-      </c>
-      <c r="O7" s="144" t="s">
-        <v>292</v>
+        <v>285</v>
+      </c>
+      <c r="N7" s="133" t="s">
+        <v>288</v>
+      </c>
+      <c r="O7" s="133" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
@@ -9612,7 +9565,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E8">
         <v>3000</v>
@@ -9621,29 +9574,29 @@
         <v>45000</v>
       </c>
       <c r="G8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I8" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>1</v>
       </c>
-      <c r="K8" s="121" t="s">
-        <v>271</v>
+      <c r="K8" s="134" t="s">
+        <v>270</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M8" t="s">
+        <v>297</v>
+      </c>
+      <c r="N8" s="133" t="s">
         <v>298</v>
       </c>
-      <c r="N8" s="144" t="s">
-        <v>299</v>
-      </c>
-      <c r="O8" s="144" t="s">
-        <v>297</v>
+      <c r="O8" s="133" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.25">
@@ -9651,7 +9604,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E9">
         <v>2000</v>
@@ -9660,27 +9613,27 @@
         <v>15000</v>
       </c>
       <c r="G9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I9" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>1</v>
       </c>
-      <c r="K9" s="121"/>
+      <c r="K9" s="134"/>
       <c r="L9" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M9" t="s">
-        <v>301</v>
-      </c>
-      <c r="N9" s="144" t="s">
+        <v>300</v>
+      </c>
+      <c r="N9" s="133" t="s">
+        <v>298</v>
+      </c>
+      <c r="O9" s="133" t="s">
         <v>299</v>
-      </c>
-      <c r="O9" s="144" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="10" spans="3:15" x14ac:dyDescent="0.25">
@@ -9688,7 +9641,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E10">
         <v>3200</v>
@@ -9697,27 +9650,27 @@
         <v>150000</v>
       </c>
       <c r="G10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I10" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>1</v>
       </c>
-      <c r="K10" s="121"/>
+      <c r="K10" s="134"/>
       <c r="L10" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M10" t="s">
-        <v>303</v>
-      </c>
-      <c r="N10" s="144" t="s">
-        <v>299</v>
-      </c>
-      <c r="O10" s="144" t="s">
-        <v>297</v>
+        <v>302</v>
+      </c>
+      <c r="N10" s="133" t="s">
+        <v>298</v>
+      </c>
+      <c r="O10" s="133" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.25">
@@ -9725,7 +9678,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E11">
         <v>5800</v>
@@ -9734,27 +9687,27 @@
         <v>125999</v>
       </c>
       <c r="G11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I11" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>0</v>
       </c>
-      <c r="K11" s="121"/>
+      <c r="K11" s="134"/>
       <c r="L11" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M11" t="s">
-        <v>302</v>
-      </c>
-      <c r="N11" s="144" t="s">
-        <v>299</v>
-      </c>
-      <c r="O11" s="144" t="s">
-        <v>304</v>
+        <v>301</v>
+      </c>
+      <c r="N11" s="133" t="s">
+        <v>298</v>
+      </c>
+      <c r="O11" s="133" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.25">
@@ -9762,7 +9715,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E12">
         <v>3500</v>
@@ -9771,27 +9724,27 @@
         <v>65000</v>
       </c>
       <c r="G12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I12" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>1</v>
       </c>
-      <c r="K12" s="121"/>
+      <c r="K12" s="134"/>
       <c r="L12" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M12" t="s">
+        <v>304</v>
+      </c>
+      <c r="N12" s="133" t="s">
+        <v>298</v>
+      </c>
+      <c r="O12" s="133" t="s">
         <v>305</v>
-      </c>
-      <c r="N12" s="144" t="s">
-        <v>299</v>
-      </c>
-      <c r="O12" s="144" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.25">
@@ -9799,7 +9752,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E13">
         <v>8000</v>
@@ -9808,27 +9761,27 @@
         <v>2000</v>
       </c>
       <c r="G13" t="s">
+        <v>254</v>
+      </c>
+      <c r="H13" t="s">
         <v>255</v>
-      </c>
-      <c r="H13" t="s">
-        <v>256</v>
       </c>
       <c r="I13" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
         <v>0</v>
       </c>
-      <c r="K13" s="121"/>
+      <c r="K13" s="134"/>
       <c r="L13" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M13" t="s">
+        <v>306</v>
+      </c>
+      <c r="N13" s="133" t="s">
+        <v>298</v>
+      </c>
+      <c r="O13" s="133" t="s">
         <v>307</v>
-      </c>
-      <c r="N13" s="144" t="s">
-        <v>299</v>
-      </c>
-      <c r="O13" s="144" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
@@ -9836,7 +9789,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E14">
         <v>25000</v>
@@ -9845,10 +9798,10 @@
         <v>15000</v>
       </c>
       <c r="G14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I14" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
@@ -9860,7 +9813,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E15">
         <v>25000</v>
@@ -9869,10 +9822,10 @@
         <v>35000</v>
       </c>
       <c r="G15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I15" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
@@ -9884,7 +9837,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E16">
         <v>5400</v>
@@ -9893,10 +9846,10 @@
         <v>85999</v>
       </c>
       <c r="G16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I16" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
@@ -9908,7 +9861,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E17">
         <v>2000</v>
@@ -9917,10 +9870,10 @@
         <v>95600</v>
       </c>
       <c r="G17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I17" t="b">
         <f>Tabla2[[#This Row],[stock]]&lt;=5000</f>
@@ -9960,7 +9913,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="verdadero">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="verdadero">
       <formula>NOT(ISERROR(SEARCH("verdadero",I2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Filtros y Tipos de graficos
</commit_message>
<xml_diff>
--- a/introduccion.xlsx
+++ b/introduccion.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\excel-x15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4D3614-EE57-4A07-8FB7-C8B244B3C988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089FCF54-B27F-4977-86B2-C37EC955B539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="1" r:id="rId1"/>
     <sheet name="listas" sheetId="2" r:id="rId2"/>
     <sheet name="f(x)" sheetId="3" r:id="rId3"/>
+    <sheet name="filtros" sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="140">
   <si>
     <t>Tipos</t>
   </si>
@@ -385,6 +386,99 @@
   </si>
   <si>
     <t>El contenido no cabe en la celda</t>
+  </si>
+  <si>
+    <t>es igual a</t>
+  </si>
+  <si>
+    <t>es menor que</t>
+  </si>
+  <si>
+    <t>es menor o igual a</t>
+  </si>
+  <si>
+    <t>es mayor que</t>
+  </si>
+  <si>
+    <t>es mayor o igual a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es igual a </t>
+  </si>
+  <si>
+    <t>contiene</t>
+  </si>
+  <si>
+    <t>no contiene</t>
+  </si>
+  <si>
+    <t>empieza por</t>
+  </si>
+  <si>
+    <t>termina con</t>
+  </si>
+  <si>
+    <t>No es igual a</t>
+  </si>
+  <si>
+    <t>Entre</t>
+  </si>
+  <si>
+    <t>referencia</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>2 Y 4</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>1,2,4,5,6,7</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>4,5,6,7</t>
+  </si>
+  <si>
+    <t>3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>2,3,4</t>
+  </si>
+  <si>
+    <t>valor</t>
+  </si>
+  <si>
+    <t>alfa, bravo, charlie, delta</t>
+  </si>
+  <si>
+    <t>alfa</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>bravo, charlie, delta</t>
+  </si>
+  <si>
+    <t>charlie, delta</t>
+  </si>
+  <si>
+    <t>alfa, bravo</t>
+  </si>
+  <si>
+    <t>alfa, delta</t>
   </si>
 </sst>
 </file>
@@ -399,7 +493,7 @@
     <numFmt numFmtId="167" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="[$€-2]\ #,##0.00"/>
     <numFmt numFmtId="169" formatCode="[$-2C0A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
-    <numFmt numFmtId="171" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="170" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -591,7 +685,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -695,13 +789,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="40% - Énfasis6" xfId="1" builtinId="51"/>
@@ -715,7 +815,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="9" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -739,6 +849,32 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EEC6AD2A-72FF-4680-9EF3-C2D11F01182E}" name="Tabla1" displayName="Tabla1" ref="A1:D8" totalsRowShown="0">
+  <autoFilter ref="A1:D8" xr:uid="{EEC6AD2A-72FF-4680-9EF3-C2D11F01182E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{EA6C3CAF-FB06-48FD-826F-9ACD5BB921A9}" name="Numero"/>
+    <tableColumn id="4" xr3:uid="{556D6157-E57C-44AB-A177-96B4714CA3E8}" name="valor" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{66EF1D8B-6C80-4F9C-90D2-9B94D5695E1D}" name="referencia" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{FE5AF678-CBCB-4B16-B981-A8578600942A}" name="resultado" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFD16820-0B6A-4732-84CC-3A8DC1480203}" name="Tabla2" displayName="Tabla2" ref="A10:D16" totalsRowShown="0">
+  <autoFilter ref="A10:D16" xr:uid="{BFD16820-0B6A-4732-84CC-3A8DC1480203}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C90747EF-6B89-48CB-94E5-F6FFCE4BBBDB}" name="Texto"/>
+    <tableColumn id="2" xr3:uid="{1B33FF03-35E1-48B8-ACD2-AB2C1A363A8D}" name="Valor"/>
+    <tableColumn id="3" xr3:uid="{6764C023-BE86-4536-A67B-85F2A882EB1B}" name="referencia"/>
+    <tableColumn id="4" xr3:uid="{CF8F8CDC-56B2-4730-AB17-18E30DDFC3F9}" name="Resultado"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1939,7 +2075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -1961,19 +2097,19 @@
       <c r="A1" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="F1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
       <c r="K1" t="s">
         <v>86</v>
       </c>
@@ -2156,7 +2292,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K7" s="59">
+      <c r="K7" s="57">
         <v>33346</v>
       </c>
       <c r="L7" t="s">
@@ -2170,4 +2306,244 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE41BFDD-BABC-49DE-937D-B2ACC3FCC68D}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="61">
+        <v>3</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="61">
+        <v>3</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="61">
+        <v>3</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="61">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="61">
+        <v>3</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="61">
+        <v>3</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="61" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="61">
+        <v>3</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="61" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ejercicios Subtotales y Operaciones Conjunto
</commit_message>
<xml_diff>
--- a/introduccion.xlsx
+++ b/introduccion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xav-j12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{543F48E0-8F2F-400F-85AF-902F602466DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E636B6-B1C5-490F-B11D-9991DE8665CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{BFB0CF28-7797-46CE-98B8-81D14DF3A489}"/>
   </bookViews>
@@ -238,7 +238,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -306,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -322,7 +322,7 @@
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="7">
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -333,26 +333,10 @@
       <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BC2E6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
@@ -384,14 +368,14 @@
     <tableColumn id="2" xr3:uid="{F9786D07-A25E-46C4-8F4C-B1F74B14B6B7}" name="apellido"/>
     <tableColumn id="3" xr3:uid="{FCCC3292-CE00-46E4-99EF-A7B83DE3E0D4}" name="nombre"/>
     <tableColumn id="4" xr3:uid="{FC499D72-DF7E-4830-BC33-62AA7AA4E98D}" name="cuil"/>
-    <tableColumn id="5" xr3:uid="{B4AA7946-4A8E-4BD2-ACD2-0F203177260B}" name="nacimiento" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{BAEFA1B4-2343-469D-9B64-5970EFC08CDD}" name="g" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{B4AA7946-4A8E-4BD2-ACD2-0F203177260B}" name="nacimiento" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{BAEFA1B4-2343-469D-9B64-5970EFC08CDD}" name="g" dataDxfId="5">
       <calculatedColumnFormula>LEFT(clientes[[#This Row],[cuil]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{84DE9DBC-2D64-4B7C-8C7D-9559321338F2}" name="documento" dataDxfId="5" dataCellStyle="Millares">
+    <tableColumn id="15" xr3:uid="{84DE9DBC-2D64-4B7C-8C7D-9559321338F2}" name="documento" dataDxfId="4" dataCellStyle="Millares">
       <calculatedColumnFormula>MID(clientes[[#This Row],[cuil]],4,8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3CFA528C-5846-49FA-BE4E-FBBD381023D2}" name="edad" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{3CFA528C-5846-49FA-BE4E-FBBD381023D2}" name="edad" dataDxfId="3">
       <calculatedColumnFormula>(hoy-E2)/365</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{BFE4F650-E152-4B99-A905-3D8E7294215D}" name="direccion"/>
@@ -803,15 +787,15 @@
         <v>85495939</v>
       </c>
       <c r="H2" s="3">
-        <f ca="1">(hoy-E2)/365</f>
-        <v>21.167123287671235</v>
+        <f t="shared" ref="H2:H12" ca="1" si="0">(hoy-E2)/365</f>
+        <v>21.186301369863013</v>
       </c>
       <c r="J2" t="s">
         <v>47</v>
       </c>
       <c r="M2" s="1">
         <f ca="1">TODAY()</f>
-        <v>44875</v>
+        <v>44882</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -839,8 +823,8 @@
         <v>82491289</v>
       </c>
       <c r="H3" s="3">
-        <f ca="1">(hoy-E3)/365</f>
-        <v>24.079452054794519</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24.098630136986301</v>
       </c>
       <c r="J3" t="s">
         <v>45</v>
@@ -871,8 +855,8 @@
         <v>92918234</v>
       </c>
       <c r="H4" s="3">
-        <f ca="1">(hoy-E4)/365</f>
-        <v>46.493150684931507</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>46.512328767123286</v>
       </c>
       <c r="J4" t="s">
         <v>44</v>
@@ -903,8 +887,8 @@
         <v>38109230</v>
       </c>
       <c r="H5" s="3">
-        <f ca="1">(hoy-E5)/365</f>
-        <v>26.715068493150685</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26.734246575342464</v>
       </c>
       <c r="J5" t="s">
         <v>43</v>
@@ -935,8 +919,8 @@
         <v>24759283</v>
       </c>
       <c r="H6" s="3">
-        <f ca="1">(hoy-E6)/365</f>
-        <v>53.282191780821918</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>53.301369863013697</v>
       </c>
       <c r="J6" t="s">
         <v>44</v>
@@ -967,8 +951,8 @@
         <v>12834917</v>
       </c>
       <c r="H7" s="3">
-        <f ca="1">(hoy-E7)/365</f>
-        <v>91.920547945205485</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>91.939726027397256</v>
       </c>
       <c r="J7" t="s">
         <v>42</v>
@@ -999,8 +983,8 @@
         <v>35336446</v>
       </c>
       <c r="H8" s="3">
-        <f ca="1">(hoy-E8)/365</f>
-        <v>31.586301369863012</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>31.605479452054794</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
@@ -1037,8 +1021,8 @@
         <v>38885460</v>
       </c>
       <c r="H9" s="3">
-        <f ca="1">(hoy-E9)/365</f>
-        <v>29.098630136986301</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>29.117808219178084</v>
       </c>
       <c r="J9" t="s">
         <v>42</v>
@@ -1069,8 +1053,8 @@
         <v>43892348</v>
       </c>
       <c r="H10" s="3">
-        <f ca="1">(hoy-E10)/365</f>
-        <v>18.87123287671233</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>18.890410958904109</v>
       </c>
       <c r="J10" t="s">
         <v>46</v>
@@ -1101,8 +1085,8 @@
         <v>28309239</v>
       </c>
       <c r="H11" s="3">
-        <f ca="1">(hoy-E11)/365</f>
-        <v>36.334246575342469</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36.353424657534248</v>
       </c>
       <c r="J11" t="s">
         <v>43</v>
@@ -1133,8 +1117,8 @@
         <v>27381823</v>
       </c>
       <c r="H12" s="3">
-        <f ca="1">(hoy-E12)/365</f>
-        <v>52.375342465753427</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>52.394520547945206</v>
       </c>
       <c r="J12" t="s">
         <v>12</v>
@@ -1175,7 +1159,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Formulas, funciones y errores
</commit_message>
<xml_diff>
--- a/introduccion.xlsx
+++ b/introduccion.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xls-v10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E59C7E7-B946-4045-AE06-60E66816AFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEAA19B-E171-4E55-92EF-2BC31E83A4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2B3C686B-3C6E-4EC4-BBA6-231B205C55CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{2B3C686B-3C6E-4EC4-BBA6-231B205C55CD}"/>
   </bookViews>
   <sheets>
     <sheet name="formatos" sheetId="1" r:id="rId1"/>
+    <sheet name="series" sheetId="2" r:id="rId2"/>
+    <sheet name="f(x)" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,8 +38,45 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="88">
   <si>
     <t>texto</t>
   </si>
@@ -73,6 +115,231 @@
   </si>
   <si>
     <t>científica</t>
+  </si>
+  <si>
+    <t>Rangos</t>
+  </si>
+  <si>
+    <t>Columna</t>
+  </si>
+  <si>
+    <t>Fila</t>
+  </si>
+  <si>
+    <t>Celda</t>
+  </si>
+  <si>
+    <t>Conjunto</t>
+  </si>
+  <si>
+    <t>Relativos</t>
+  </si>
+  <si>
+    <t>Absolutos</t>
+  </si>
+  <si>
+    <t>A:A; A1:A10</t>
+  </si>
+  <si>
+    <t>1:1; A1:C1</t>
+  </si>
+  <si>
+    <t>A1; B1; C1</t>
+  </si>
+  <si>
+    <t>A1:C10</t>
+  </si>
+  <si>
+    <t>$A:$A</t>
+  </si>
+  <si>
+    <t>$1:$1</t>
+  </si>
+  <si>
+    <t>$A$1</t>
+  </si>
+  <si>
+    <t>$A$1:$C$10</t>
+  </si>
+  <si>
+    <t>dias</t>
+  </si>
+  <si>
+    <t>meses</t>
+  </si>
+  <si>
+    <t>numeros</t>
+  </si>
+  <si>
+    <t>intervalos</t>
+  </si>
+  <si>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t>sábado</t>
+  </si>
+  <si>
+    <t>domingo</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t>miércoles</t>
+  </si>
+  <si>
+    <t>jueves</t>
+  </si>
+  <si>
+    <t>noviembre</t>
+  </si>
+  <si>
+    <t>diciembre</t>
+  </si>
+  <si>
+    <t>enero</t>
+  </si>
+  <si>
+    <t>febrero</t>
+  </si>
+  <si>
+    <t>marzo</t>
+  </si>
+  <si>
+    <t>abril</t>
+  </si>
+  <si>
+    <t>mayo</t>
+  </si>
+  <si>
+    <t>junio</t>
+  </si>
+  <si>
+    <t>julio</t>
+  </si>
+  <si>
+    <t>agosto</t>
+  </si>
+  <si>
+    <t>septiembre</t>
+  </si>
+  <si>
+    <t>octubre</t>
+  </si>
+  <si>
+    <t>textos</t>
+  </si>
+  <si>
+    <t>factura-A-0001</t>
+  </si>
+  <si>
+    <t>factura-A-0002</t>
+  </si>
+  <si>
+    <t>factura-A-0003</t>
+  </si>
+  <si>
+    <t>factura-A-0004</t>
+  </si>
+  <si>
+    <t>factura-A-0005</t>
+  </si>
+  <si>
+    <t>factura-A-0006</t>
+  </si>
+  <si>
+    <t>factura-A-0007</t>
+  </si>
+  <si>
+    <t>factura-A-0008</t>
+  </si>
+  <si>
+    <t>factura-A-0009</t>
+  </si>
+  <si>
+    <t>factura-A-0010</t>
+  </si>
+  <si>
+    <t>factura-A-0011</t>
+  </si>
+  <si>
+    <t>factura-A-0012</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>valor 1</t>
+  </si>
+  <si>
+    <t>valor 2</t>
+  </si>
+  <si>
+    <t>resultado</t>
+  </si>
+  <si>
+    <t>suma</t>
+  </si>
+  <si>
+    <t>resta</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>producto</t>
+  </si>
+  <si>
+    <t>potencia</t>
+  </si>
+  <si>
+    <t>Operaciones aritmeticas que utilizan los valores de las celdas, los cuales deben ser validos, ya que de lo contrario arrojara un error</t>
+  </si>
+  <si>
+    <t>contar</t>
+  </si>
+  <si>
+    <t>residuo</t>
+  </si>
+  <si>
+    <t>Palabras reservadas que se utilizan para realizar una operación, reciben argumentos y suelen ignorar los valores que no sean validos</t>
+  </si>
+  <si>
+    <t>ERRORES</t>
+  </si>
+  <si>
+    <t>FUNCIONES</t>
+  </si>
+  <si>
+    <t>FORMULAS</t>
+  </si>
+  <si>
+    <t>tipo de dato erroneo</t>
+  </si>
+  <si>
+    <t>division entre 0</t>
+  </si>
+  <si>
+    <t>referencia no encontrada</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>contenido supera el limite</t>
+  </si>
+  <si>
+    <t>Valores que indican algun inconveniente con la formula de la celda que lo contiene, normalmente incluyen un detalle que indica el motivo del mismo y como resoverlo.</t>
+  </si>
+  <si>
+    <t>celda demasiado angosta</t>
   </si>
 </sst>
 </file>
@@ -82,14 +349,14 @@
   <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="171" formatCode="_-[$$-2C0A]\ * #,##0_-;\-[$$-2C0A]\ * #,##0_-;_-[$$-2C0A]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="174" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="176" formatCode="[$-2C0A]h:mm:ss\ AM/PM;@"/>
-    <numFmt numFmtId="177" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="_-[$$-2C0A]\ * #,##0_-;\-[$$-2C0A]\ * #,##0_-;_-[$$-2C0A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="[$-2C0A]h:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +371,81 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,26 +457,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="11"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="13"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="12"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="14">
+    <cellStyle name="40% - Énfasis1" xfId="5" builtinId="31"/>
+    <cellStyle name="40% - Énfasis2" xfId="7" builtinId="35"/>
+    <cellStyle name="40% - Énfasis3" xfId="9" builtinId="39"/>
+    <cellStyle name="40% - Énfasis4" xfId="11" builtinId="43"/>
+    <cellStyle name="40% - Énfasis6" xfId="13" builtinId="51"/>
+    <cellStyle name="Énfasis1" xfId="4" builtinId="29"/>
+    <cellStyle name="Énfasis2" xfId="6" builtinId="33"/>
+    <cellStyle name="Énfasis3" xfId="8" builtinId="37"/>
+    <cellStyle name="Énfasis4" xfId="10" builtinId="41"/>
+    <cellStyle name="Énfasis6" xfId="12" builtinId="49"/>
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -158,6 +537,81 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="estadisticas"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>8</v>
+    <v>0</v>
+    <v>3</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="colOffset" t="i"/>
+    <k n="errorType" t="i"/>
+    <k n="rwOffset" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,19 +911,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAC9467-D7D2-43FD-A5FA-A2B7A0C40AC7}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -479,8 +935,17 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -490,8 +955,17 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -501,8 +975,17 @@
       <c r="C3">
         <v>3.14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -513,8 +996,17 @@
         <v>33346</v>
       </c>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -525,8 +1017,17 @@
         <v>0.3263888888888889</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -537,7 +1038,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -548,7 +1049,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -559,7 +1060,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -576,4 +1077,738 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849FD030-11BB-4D13-9822-3406A3DE4631}">
+  <dimension ref="A1:S13"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+      <c r="D2" s="15">
+        <v>30</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2</v>
+      </c>
+      <c r="D3" s="15">
+        <v>25</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="14">
+        <v>1</v>
+      </c>
+      <c r="I3" s="14">
+        <v>2</v>
+      </c>
+      <c r="J3" s="14">
+        <v>3</v>
+      </c>
+      <c r="K3" s="14">
+        <v>4</v>
+      </c>
+      <c r="L3" s="14">
+        <v>5</v>
+      </c>
+      <c r="M3" s="14">
+        <v>6</v>
+      </c>
+      <c r="N3" s="14">
+        <v>7</v>
+      </c>
+      <c r="O3" s="14">
+        <v>8</v>
+      </c>
+      <c r="P3" s="14">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>10</v>
+      </c>
+      <c r="R3" s="14">
+        <v>11</v>
+      </c>
+      <c r="S3" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="14">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <v>20</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="15">
+        <v>30</v>
+      </c>
+      <c r="I4" s="15">
+        <v>25</v>
+      </c>
+      <c r="J4" s="15">
+        <v>20</v>
+      </c>
+      <c r="K4" s="15">
+        <v>15</v>
+      </c>
+      <c r="L4" s="15">
+        <v>10</v>
+      </c>
+      <c r="M4" s="15">
+        <v>5</v>
+      </c>
+      <c r="N4" s="15">
+        <v>0</v>
+      </c>
+      <c r="O4" s="15">
+        <v>-5</v>
+      </c>
+      <c r="P4" s="15">
+        <v>-10</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>-15</v>
+      </c>
+      <c r="R4" s="15">
+        <v>-20</v>
+      </c>
+      <c r="S4" s="15">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="14">
+        <v>4</v>
+      </c>
+      <c r="D5" s="15">
+        <v>15</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="14">
+        <v>5</v>
+      </c>
+      <c r="D6" s="15">
+        <v>10</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="14">
+        <v>6</v>
+      </c>
+      <c r="D7" s="15">
+        <v>5</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="14">
+        <v>7</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="14">
+        <v>8</v>
+      </c>
+      <c r="D9" s="15">
+        <v>-5</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="14">
+        <v>9</v>
+      </c>
+      <c r="D10" s="15">
+        <v>-10</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="14">
+        <v>10</v>
+      </c>
+      <c r="D11" s="15">
+        <v>-15</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="14">
+        <v>11</v>
+      </c>
+      <c r="D12" s="15">
+        <v>-20</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="14">
+        <v>12</v>
+      </c>
+      <c r="D13" s="15">
+        <v>-25</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A781DEF4-4409-4A93-A784-F4AB839DC094}">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="F1" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="K1" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" s="22"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+    </row>
+    <row r="2" spans="1:14" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="F2" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="K2" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="23"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f>B5+C5</f>
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f>SUM(F5:H5)</f>
+        <v>7</v>
+      </c>
+      <c r="K5" t="e">
+        <f>I5+K4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f>B6-C6</f>
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <f>COUNT(F6:H6)</f>
+        <v>2</v>
+      </c>
+      <c r="K6" t="e">
+        <f>[1]estadisticas!A1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f>B7*C7</f>
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <f>PRODUCT(F7:H7)</f>
+        <v>10</v>
+      </c>
+      <c r="K7" t="e">
+        <f>G8/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f>B8/C8</f>
+        <v>2.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <f>MOD(G8,H8)</f>
+        <v>1</v>
+      </c>
+      <c r="K8" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="K8" ca="1">A:A</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L8" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f>B9^C9</f>
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <f>POWER(G9,H9)</f>
+        <v>25</v>
+      </c>
+      <c r="K9" s="24">
+        <f>2^128</f>
+        <v>3.4028236692093846E+38</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K2:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>